<commit_message>
first services excel semi update
</commit_message>
<xml_diff>
--- a/services/services.xlsx
+++ b/services/services.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roise\Documents\Apam ciber\leaks\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC46CA3-8DF5-455D-8191-3F45A0FDA0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99AD2FA-73C0-49FB-90AC-080A696EFCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Services" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="280">
   <si>
     <t>Website</t>
   </si>
@@ -872,6 +872,12 @@
   </si>
   <si>
     <t>access tlf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>gog.com</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1622,7 @@
     <tableColumn id="27" xr3:uid="{02F2CE9F-3AA5-4646-98D5-CB066ED14A49}" name="Surname" dataCellStyle="Bad"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="birth date"/>
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="gender"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Profile photo"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Profile photo" dataCellStyle="Bad"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="email"/>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="tlf"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="nacionality"/>
@@ -1905,18 +1911,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="2.28515625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
@@ -1928,7 +1934,9 @@
     <col min="14" max="14" width="8.85546875" customWidth="1"/>
     <col min="15" max="15" width="8.85546875" style="16" customWidth="1"/>
     <col min="16" max="16" width="11.140625" customWidth="1"/>
-    <col min="17" max="21" width="8.85546875" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="16" customWidth="1"/>
+    <col min="19" max="21" width="8.85546875" customWidth="1"/>
     <col min="22" max="22" width="9.7109375" customWidth="1"/>
     <col min="23" max="23" width="9.28515625" customWidth="1"/>
     <col min="24" max="24" width="9.28515625" style="16" customWidth="1"/>
@@ -1992,7 +2000,7 @@
       <c r="Q1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="16" t="s">
         <v>273</v>
       </c>
       <c r="S1" s="1" t="s">
@@ -2053,22 +2061,26 @@
       <c r="H2" s="1">
         <v>1</v>
       </c>
-      <c r="L2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1"/>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="O2"/>
+      <c r="Q2">
+        <v>1</v>
+      </c>
+      <c r="R2"/>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="X2"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1">
         <v>1</v>
@@ -2107,28 +2119,29 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
-        <v>1</v>
-      </c>
-      <c r="P3" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>1</v>
-      </c>
-      <c r="R3" s="1">
-        <v>1</v>
-      </c>
-      <c r="S3" s="1">
-        <v>1</v>
-      </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
+      <c r="I3"/>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3"/>
+      <c r="M3"/>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3"/>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="X3"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
@@ -2159,22 +2172,27 @@
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="L4" s="1">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1">
-        <v>1</v>
-      </c>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4"/>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="O4"/>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="X4"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1">
         <v>1</v>
@@ -2189,125 +2207,124 @@
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>6</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="N5" s="1">
-        <v>1</v>
-      </c>
-      <c r="P5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>1</v>
-      </c>
-      <c r="R5" s="1">
-        <v>1</v>
-      </c>
-      <c r="S5" s="1">
-        <v>1</v>
-      </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1">
-        <v>1</v>
-      </c>
-      <c r="W5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5"/>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="O5"/>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6">
         <v>8</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="L6" s="1">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1">
-        <v>1</v>
-      </c>
-      <c r="P6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>1</v>
-      </c>
-      <c r="R6" s="1">
-        <v>1</v>
-      </c>
-      <c r="S6" s="1">
-        <v>1</v>
-      </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1">
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6"/>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="O6"/>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="X6"/>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>204</v>
       </c>
       <c r="B7" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>133</v>
       </c>
       <c r="F7">
@@ -2316,12 +2333,21 @@
       <c r="G7" t="s">
         <v>56</v>
       </c>
+      <c r="I7"/>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7"/>
       <c r="L7">
         <v>1</v>
       </c>
+      <c r="M7"/>
       <c r="N7">
         <v>1</v>
       </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
       <c r="P7">
         <v>1</v>
       </c>
@@ -2343,6 +2369,7 @@
       <c r="W7">
         <v>1</v>
       </c>
+      <c r="X7"/>
       <c r="Y7">
         <v>1</v>
       </c>
@@ -2351,13 +2378,13 @@
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>226</v>
       </c>
       <c r="B8" t="s">
         <v>234</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>133</v>
       </c>
       <c r="F8">
@@ -2366,21 +2393,30 @@
       <c r="G8" t="s">
         <v>27</v>
       </c>
+      <c r="I8"/>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8"/>
+      <c r="M8"/>
+      <c r="O8"/>
+      <c r="R8"/>
       <c r="S8">
         <v>1</v>
       </c>
+      <c r="X8"/>
       <c r="AB8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>227</v>
       </c>
       <c r="B9" t="s">
         <v>235</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>133</v>
       </c>
       <c r="F9">
@@ -2389,15 +2425,23 @@
       <c r="G9" t="s">
         <v>27</v>
       </c>
+      <c r="I9"/>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9"/>
+      <c r="M9"/>
       <c r="N9">
         <v>1</v>
       </c>
+      <c r="O9"/>
       <c r="P9">
         <v>1</v>
       </c>
       <c r="Q9">
         <v>1</v>
       </c>
+      <c r="R9"/>
       <c r="S9">
         <v>1</v>
       </c>
@@ -2407,58 +2451,56 @@
       <c r="W9">
         <v>1</v>
       </c>
+      <c r="X9"/>
       <c r="AB9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>156</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1">
+      <c r="F10">
         <v>8</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="1"/>
-      <c r="L10" s="1">
-        <v>1</v>
-      </c>
-      <c r="N10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1">
-        <v>1</v>
-      </c>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
+      <c r="I10"/>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10"/>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10"/>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="X10"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>229</v>
       </c>
       <c r="B11" t="s">
         <v>237</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>133</v>
       </c>
       <c r="F11">
@@ -2467,517 +2509,571 @@
       <c r="G11" t="s">
         <v>27</v>
       </c>
+      <c r="I11"/>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11"/>
       <c r="L11">
         <v>1</v>
       </c>
-      <c r="N11">
-        <v>1</v>
-      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="O11"/>
+      <c r="R11"/>
       <c r="S11">
         <v>1</v>
       </c>
       <c r="V11">
         <v>1</v>
       </c>
+      <c r="X11"/>
       <c r="AA11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>216</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" t="s">
         <v>217</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>133</v>
       </c>
       <c r="F12">
         <v>9</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" t="s">
         <v>27</v>
       </c>
-      <c r="L12" s="7">
-        <v>1</v>
-      </c>
-      <c r="N12" s="7">
-        <v>1</v>
-      </c>
-      <c r="P12" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="7">
-        <v>1</v>
-      </c>
-      <c r="R12" s="7">
-        <v>1</v>
-      </c>
-      <c r="S12" s="7">
-        <v>1</v>
-      </c>
-      <c r="T12" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="7">
+      <c r="I12"/>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12"/>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12"/>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="X12"/>
+      <c r="Z12">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>151</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>152</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
+      <c r="F13">
         <v>10</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" t="s">
         <v>153</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="N13" s="1">
-        <v>1</v>
-      </c>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1">
-        <v>1</v>
-      </c>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1">
-        <v>1</v>
-      </c>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
+      <c r="I13"/>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13"/>
+      <c r="M13"/>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="R13"/>
+      <c r="S13">
+        <v>1</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>1</v>
+      </c>
+      <c r="X13"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>160</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>161</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>133</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
+      <c r="F14">
         <v>8</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="1">
-        <v>1</v>
-      </c>
-      <c r="L14" s="1">
-        <v>1</v>
-      </c>
-      <c r="N14" s="1">
-        <v>1</v>
-      </c>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1">
-        <v>1</v>
-      </c>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1">
-        <v>1</v>
-      </c>
-      <c r="T14" s="1">
-        <v>1</v>
-      </c>
-      <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14"/>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14"/>
+      <c r="AA14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>145</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>146</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
+      <c r="F15">
         <v>8</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" t="s">
         <v>101</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="L15" s="1">
-        <v>1</v>
-      </c>
-      <c r="N15" s="1">
-        <v>1</v>
-      </c>
-      <c r="P15" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1">
-        <v>1</v>
-      </c>
-      <c r="S15" s="1">
-        <v>1</v>
-      </c>
-      <c r="T15" s="1">
-        <v>1</v>
-      </c>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
+      <c r="I15"/>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15"/>
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+      <c r="T15">
+        <v>1</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>207</v>
       </c>
       <c r="B16" t="s">
         <v>162</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" t="s">
         <v>44</v>
       </c>
       <c r="F16">
         <v>8</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" t="s">
         <v>27</v>
       </c>
-      <c r="H16" s="7">
-        <v>1</v>
-      </c>
-      <c r="L16" s="7">
-        <v>1</v>
-      </c>
-      <c r="N16" s="7">
-        <v>1</v>
-      </c>
-      <c r="S16" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z16" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16"/>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16"/>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="O16"/>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="X16"/>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17">
         <v>12</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="L17" s="1">
-        <v>1</v>
-      </c>
-      <c r="N17" s="1">
-        <v>1</v>
-      </c>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1">
-        <v>1</v>
-      </c>
-      <c r="S17" s="1">
-        <v>1</v>
-      </c>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="I17"/>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17"/>
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17"/>
+      <c r="N17">
+        <v>1</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="X17"/>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>220</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" t="s">
         <v>221</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" t="s">
         <v>44</v>
       </c>
       <c r="F18">
         <v>6</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" t="s">
         <v>56</v>
       </c>
-      <c r="L18" s="7">
-        <v>1</v>
-      </c>
-      <c r="N18" s="7">
-        <v>1</v>
-      </c>
-      <c r="R18" s="7">
-        <v>1</v>
-      </c>
-      <c r="S18" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="I18"/>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18"/>
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18"/>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="X18"/>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>149</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>150</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1">
+      <c r="F19">
         <v>6</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="1">
-        <v>1</v>
-      </c>
-      <c r="L19" s="1">
-        <v>1</v>
-      </c>
-      <c r="N19" s="1">
-        <v>1</v>
-      </c>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1">
-        <v>1</v>
-      </c>
-      <c r="T19" s="1">
-        <v>1</v>
-      </c>
-      <c r="U19" s="1">
-        <v>1</v>
-      </c>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="1"/>
-      <c r="AB19" s="1"/>
-      <c r="AC19" s="1"/>
-      <c r="AD19" s="1"/>
-    </row>
-    <row r="20" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19"/>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19"/>
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19"/>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>278</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>1</v>
+      </c>
+      <c r="U19">
+        <v>1</v>
+      </c>
+      <c r="X19"/>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>136</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>137</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1">
+      <c r="F20">
         <v>6</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="L20" s="1">
-        <v>1</v>
-      </c>
-      <c r="N20" s="1">
-        <v>1</v>
-      </c>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1">
-        <v>1</v>
-      </c>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1">
-        <v>1</v>
-      </c>
-      <c r="W20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="1"/>
-      <c r="AC20" s="1"/>
-      <c r="AD20" s="1"/>
-    </row>
-    <row r="21" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="I20"/>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20"/>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20"/>
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+      <c r="R20"/>
+      <c r="S20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="X20"/>
+      <c r="Z20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>155</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1">
+      <c r="F21">
         <v>8</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" t="s">
         <v>27</v>
       </c>
-      <c r="H21" s="1">
-        <v>1</v>
-      </c>
-      <c r="L21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1">
-        <v>1</v>
-      </c>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-    </row>
-    <row r="22" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21"/>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21"/>
+      <c r="R21"/>
+      <c r="S21">
+        <v>1</v>
+      </c>
+      <c r="X21"/>
+      <c r="Z21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>218</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" t="s">
         <v>219</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" t="s">
         <v>44</v>
       </c>
       <c r="F22">
         <v>8</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" t="s">
         <v>101</v>
       </c>
-      <c r="N22" s="7">
-        <v>1</v>
-      </c>
-      <c r="S22" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA22" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="I22"/>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22"/>
+      <c r="M22"/>
+      <c r="O22"/>
+      <c r="R22"/>
+      <c r="S22">
+        <v>1</v>
+      </c>
+      <c r="X22"/>
+      <c r="AA22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>222</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" t="s">
         <v>223</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" t="s">
         <v>44</v>
       </c>
       <c r="F23">
         <v>8</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" t="s">
         <v>101</v>
       </c>
-      <c r="L23" s="7">
-        <v>1</v>
-      </c>
-      <c r="N23" s="7">
-        <v>1</v>
-      </c>
-      <c r="S23" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z23" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23"/>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23"/>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23"/>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="R23">
+        <v>1</v>
+      </c>
+      <c r="S23">
+        <v>1</v>
+      </c>
+      <c r="X23"/>
+      <c r="Z23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>256</v>
       </c>
@@ -2993,568 +3089,577 @@
       <c r="G24" t="s">
         <v>27</v>
       </c>
-      <c r="N24">
-        <v>1</v>
-      </c>
+      <c r="I24"/>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24"/>
+      <c r="M24">
+        <v>1</v>
+      </c>
+      <c r="O24"/>
       <c r="P24">
         <v>1</v>
       </c>
       <c r="Q24">
         <v>1</v>
       </c>
+      <c r="R24"/>
       <c r="S24">
         <v>1</v>
       </c>
       <c r="U24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="X24"/>
+    </row>
+    <row r="25" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25">
         <v>8</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="L25" s="1">
-        <v>1</v>
-      </c>
-      <c r="N25" s="1">
-        <v>1</v>
-      </c>
-      <c r="P25" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="1">
-        <v>1</v>
-      </c>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1">
-        <v>1</v>
-      </c>
-      <c r="T25" s="1">
-        <v>1</v>
-      </c>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1">
-        <v>1</v>
-      </c>
-      <c r="W25" s="1"/>
-      <c r="Y25" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD25" s="1"/>
-    </row>
-    <row r="26" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="I25"/>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25"/>
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25"/>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>1</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>1</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="V25">
+        <v>1</v>
+      </c>
+      <c r="X25"/>
+      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
+        <v>1</v>
+      </c>
+      <c r="AA25">
+        <v>1</v>
+      </c>
+      <c r="AC25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>158</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1">
+      <c r="F26">
         <v>8</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="1">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1">
-        <v>1</v>
-      </c>
-      <c r="N26" s="1">
-        <v>1</v>
-      </c>
-      <c r="P26" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="1">
-        <v>1</v>
-      </c>
-      <c r="R26" s="1"/>
-      <c r="S26" s="1">
-        <v>1</v>
-      </c>
-      <c r="T26" s="1">
-        <v>1</v>
-      </c>
-      <c r="U26" s="1"/>
-      <c r="V26" s="1"/>
-      <c r="W26" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z26" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA26" s="1"/>
-      <c r="AB26" s="1"/>
-      <c r="AC26" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD26" s="1"/>
-    </row>
-    <row r="27" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26"/>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26"/>
+      <c r="L26">
+        <v>1</v>
+      </c>
+      <c r="M26"/>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+      <c r="P26">
+        <v>1</v>
+      </c>
+      <c r="Q26">
+        <v>1</v>
+      </c>
+      <c r="R26"/>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26"/>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+      <c r="Z26">
+        <v>1</v>
+      </c>
+      <c r="AC26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E27" t="s">
         <v>46</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27">
         <v>8</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="1">
-        <v>1</v>
-      </c>
-      <c r="L27" s="1">
-        <v>1</v>
-      </c>
-      <c r="N27" s="1">
-        <v>1</v>
-      </c>
-      <c r="P27" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="1"/>
-      <c r="R27" s="1">
-        <v>1</v>
-      </c>
-      <c r="S27" s="1">
-        <v>1</v>
-      </c>
-      <c r="T27" s="1">
-        <v>1</v>
-      </c>
-      <c r="U27" s="1"/>
-      <c r="V27" s="1">
-        <v>1</v>
-      </c>
-      <c r="W27" s="1"/>
-      <c r="Y27" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z27" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA27" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB27" s="1"/>
-      <c r="AC27" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD27" s="1"/>
-    </row>
-    <row r="28" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27"/>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27"/>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27"/>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+      <c r="P27">
+        <v>1</v>
+      </c>
+      <c r="R27">
+        <v>1</v>
+      </c>
+      <c r="S27">
+        <v>1</v>
+      </c>
+      <c r="T27">
+        <v>1</v>
+      </c>
+      <c r="V27">
+        <v>1</v>
+      </c>
+      <c r="X27"/>
+      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>1</v>
+      </c>
+      <c r="AC27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
         <v>46</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28">
         <v>8</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" t="s">
         <v>27</v>
       </c>
-      <c r="H28" s="1">
-        <v>1</v>
-      </c>
-      <c r="L28" s="1">
-        <v>1</v>
-      </c>
-      <c r="N28" s="1">
-        <v>1</v>
-      </c>
-      <c r="P28" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="1">
-        <v>1</v>
-      </c>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1">
-        <v>1</v>
-      </c>
-      <c r="T28" s="1">
-        <v>1</v>
-      </c>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
-      <c r="Y28" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z28" s="1"/>
-      <c r="AA28" s="1"/>
-      <c r="AB28" s="1"/>
-      <c r="AC28" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD28" s="1"/>
-    </row>
-    <row r="29" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28"/>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28"/>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28"/>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+      <c r="P28">
+        <v>1</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28"/>
+      <c r="S28">
+        <v>1</v>
+      </c>
+      <c r="T28">
+        <v>1</v>
+      </c>
+      <c r="X28"/>
+      <c r="Y28">
+        <v>1</v>
+      </c>
+      <c r="AC28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>53</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E29" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="1">
+      <c r="F29">
         <v>6</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" t="s">
         <v>56</v>
       </c>
-      <c r="H29" s="1">
-        <v>1</v>
-      </c>
-      <c r="L29" s="1">
-        <v>1</v>
-      </c>
-      <c r="N29" s="1">
-        <v>1</v>
-      </c>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1">
-        <v>1</v>
-      </c>
-      <c r="T29" s="1">
-        <v>1</v>
-      </c>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="Y29" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z29" s="1"/>
-      <c r="AA29" s="1"/>
-      <c r="AB29" s="1"/>
-      <c r="AC29" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD29" s="1"/>
-    </row>
-    <row r="30" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29"/>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29"/>
+      <c r="L29">
+        <v>1</v>
+      </c>
+      <c r="M29"/>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29">
+        <v>1</v>
+      </c>
+      <c r="R29"/>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <v>1</v>
+      </c>
+      <c r="X29"/>
+      <c r="Y29">
+        <v>1</v>
+      </c>
+      <c r="AC29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" t="s">
         <v>63</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1">
+      <c r="F30">
         <v>8</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" t="s">
         <v>69</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1">
-        <v>1</v>
-      </c>
-      <c r="S30" s="1">
-        <v>1</v>
-      </c>
-      <c r="T30" s="1"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="1"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="1"/>
-    </row>
-    <row r="31" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="I30"/>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30"/>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="O30"/>
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="X30"/>
+    </row>
+    <row r="31" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31">
         <v>10</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="1">
-        <v>1</v>
-      </c>
-      <c r="L31" s="1"/>
-      <c r="N31" s="1">
-        <v>1</v>
-      </c>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1">
-        <v>1</v>
-      </c>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA31" s="1"/>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="1"/>
-    </row>
-    <row r="32" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31"/>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31"/>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="O31"/>
+      <c r="R31"/>
+      <c r="S31">
+        <v>1</v>
+      </c>
+      <c r="X31"/>
+      <c r="Z31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="E32" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32">
         <v>6</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" t="s">
         <v>27</v>
       </c>
-      <c r="H32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="N32" s="1">
-        <v>1</v>
-      </c>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1">
-        <v>1</v>
-      </c>
-      <c r="T32" s="1">
-        <v>1</v>
-      </c>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA32" s="1"/>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="1"/>
-    </row>
-    <row r="33" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="I32"/>
+      <c r="J32">
+        <v>1</v>
+      </c>
+      <c r="K32"/>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="O32"/>
+      <c r="R32"/>
+      <c r="S32">
+        <v>1</v>
+      </c>
+      <c r="T32">
+        <v>1</v>
+      </c>
+      <c r="X32"/>
+      <c r="Z32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" t="s">
         <v>73</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" t="s">
         <v>75</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33">
         <v>10</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" t="s">
         <v>37</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="N33" s="1">
-        <v>1</v>
-      </c>
-      <c r="P33" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>1</v>
-      </c>
-      <c r="R33" s="1">
-        <v>1</v>
-      </c>
-      <c r="S33" s="1">
-        <v>1</v>
-      </c>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1">
-        <v>1</v>
-      </c>
-      <c r="W33" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA33" s="1"/>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="1"/>
-    </row>
-    <row r="34" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="I33"/>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33"/>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="O33"/>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>1</v>
+      </c>
+      <c r="R33">
+        <v>1</v>
+      </c>
+      <c r="S33">
+        <v>1</v>
+      </c>
+      <c r="V33">
+        <v>1</v>
+      </c>
+      <c r="W33">
+        <v>1</v>
+      </c>
+      <c r="X33"/>
+      <c r="Z33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>70</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E34" t="s">
         <v>46</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34">
         <v>8</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" t="s">
         <v>27</v>
       </c>
-      <c r="H34" s="1"/>
-      <c r="L34" s="1">
-        <v>1</v>
-      </c>
-      <c r="N34" s="1"/>
-      <c r="P34" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1">
-        <v>1</v>
-      </c>
-      <c r="S34" s="1">
-        <v>1</v>
-      </c>
-      <c r="T34" s="1">
-        <v>1</v>
-      </c>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="Y34" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z34" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA34" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="1"/>
-    </row>
-    <row r="35" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="O34"/>
+      <c r="P34">
+        <v>1</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <v>1</v>
+      </c>
+      <c r="T34">
+        <v>1</v>
+      </c>
+      <c r="X34"/>
+      <c r="Y34">
+        <v>1</v>
+      </c>
+      <c r="Z34">
+        <v>1</v>
+      </c>
+      <c r="AA34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>187</v>
       </c>
       <c r="B35" t="s">
@@ -3572,15 +3677,25 @@
       <c r="G35" t="s">
         <v>56</v>
       </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35"/>
+      <c r="K35"/>
       <c r="L35">
         <v>1</v>
       </c>
+      <c r="M35"/>
       <c r="N35">
         <v>1</v>
       </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
       <c r="P35">
         <v>1</v>
       </c>
+      <c r="R35"/>
       <c r="S35">
         <v>1</v>
       </c>
@@ -3590,6 +3705,7 @@
       <c r="W35">
         <v>1</v>
       </c>
+      <c r="X35"/>
       <c r="AA35">
         <v>1</v>
       </c>
@@ -3597,8 +3713,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>184</v>
       </c>
       <c r="B36" t="s">
@@ -3622,15 +3738,25 @@
       <c r="H36">
         <v>1</v>
       </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36"/>
+      <c r="K36"/>
       <c r="L36">
         <v>1</v>
       </c>
+      <c r="M36"/>
       <c r="N36">
         <v>1</v>
       </c>
+      <c r="O36">
+        <v>1</v>
+      </c>
       <c r="P36">
         <v>1</v>
       </c>
+      <c r="R36"/>
       <c r="S36">
         <v>1</v>
       </c>
@@ -3643,6 +3769,7 @@
       <c r="W36">
         <v>1</v>
       </c>
+      <c r="X36"/>
       <c r="AA36">
         <v>1</v>
       </c>
@@ -3650,114 +3777,120 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>138</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" t="s">
         <v>139</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" t="s">
         <v>140</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1">
+      <c r="F37">
         <v>8</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" t="s">
         <v>56</v>
       </c>
-      <c r="H37" s="1">
-        <v>1</v>
-      </c>
-      <c r="L37" s="1">
-        <v>1</v>
-      </c>
-      <c r="N37" s="1">
-        <v>1</v>
-      </c>
-      <c r="P37" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="1"/>
-      <c r="R37" s="1">
-        <v>1</v>
-      </c>
-      <c r="S37" s="1">
-        <v>1</v>
-      </c>
-      <c r="T37" s="1">
-        <v>1</v>
-      </c>
-      <c r="U37" s="1">
-        <v>1</v>
-      </c>
-      <c r="V37" s="1"/>
-      <c r="W37" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y37" s="1"/>
-      <c r="Z37" s="1"/>
-      <c r="AA37" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB37" s="1">
-        <v>1</v>
-      </c>
-      <c r="AC37" s="1"/>
-      <c r="AD37" s="1"/>
-    </row>
-    <row r="38" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="I37"/>
+      <c r="J37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37"/>
+      <c r="N37">
+        <v>1</v>
+      </c>
+      <c r="O37">
+        <v>1</v>
+      </c>
+      <c r="P37">
+        <v>1</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="S37">
+        <v>1</v>
+      </c>
+      <c r="T37">
+        <v>1</v>
+      </c>
+      <c r="U37">
+        <v>1</v>
+      </c>
+      <c r="W37">
+        <v>1</v>
+      </c>
+      <c r="X37"/>
+      <c r="AA37">
+        <v>1</v>
+      </c>
+      <c r="AB37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>147</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" t="s">
         <v>140</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1">
+      <c r="F38">
         <v>7</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="1">
-        <v>1</v>
-      </c>
-      <c r="L38" s="1">
-        <v>1</v>
-      </c>
-      <c r="N38" s="1">
-        <v>1</v>
-      </c>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
-      <c r="S38" s="1">
-        <v>1</v>
-      </c>
-      <c r="T38" s="1">
-        <v>1</v>
-      </c>
-      <c r="U38" s="1"/>
-      <c r="V38" s="1"/>
-      <c r="W38" s="1"/>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA38" s="1"/>
-      <c r="AB38" s="1"/>
-      <c r="AC38" s="1"/>
-      <c r="AD38" s="1"/>
-    </row>
-    <row r="39" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38"/>
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="R38"/>
+      <c r="S38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="X38"/>
+      <c r="Z38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>189</v>
       </c>
       <c r="B39" t="s">
@@ -3778,15 +3911,25 @@
       <c r="H39">
         <v>1</v>
       </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39"/>
+      <c r="K39"/>
       <c r="L39">
         <v>1</v>
       </c>
+      <c r="M39"/>
       <c r="N39">
         <v>1</v>
       </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
       <c r="P39">
         <v>1</v>
       </c>
+      <c r="R39"/>
       <c r="S39">
         <v>1</v>
       </c>
@@ -3796,6 +3939,7 @@
       <c r="W39">
         <v>1</v>
       </c>
+      <c r="X39"/>
       <c r="AA39">
         <v>1</v>
       </c>
@@ -3803,298 +3947,320 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>82</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" t="s">
         <v>265</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E40" t="s">
         <v>46</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40">
         <v>8</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" t="s">
         <v>56</v>
       </c>
-      <c r="H40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="N40" s="1">
-        <v>1</v>
-      </c>
-      <c r="P40" s="1"/>
-      <c r="Q40" s="1"/>
-      <c r="R40" s="1">
-        <v>1</v>
-      </c>
-      <c r="S40" s="1">
-        <v>1</v>
-      </c>
-      <c r="T40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="1">
-        <v>1</v>
-      </c>
-      <c r="W40" s="1"/>
-      <c r="Y40" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z40" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA40" s="1"/>
-      <c r="AB40" s="1"/>
-      <c r="AC40" s="1"/>
-      <c r="AD40" s="1"/>
-    </row>
-    <row r="41" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40"/>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="R40">
+        <v>1</v>
+      </c>
+      <c r="S40">
+        <v>1</v>
+      </c>
+      <c r="V40">
+        <v>1</v>
+      </c>
+      <c r="X40"/>
+      <c r="Y40">
+        <v>1</v>
+      </c>
+      <c r="Z40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" t="s">
         <v>265</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" t="s">
         <v>85</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E41" t="s">
         <v>46</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41">
         <v>8</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G41" t="s">
         <v>56</v>
       </c>
-      <c r="H41" s="1"/>
-      <c r="L41" s="1"/>
-      <c r="N41" s="1">
-        <v>1</v>
-      </c>
-      <c r="P41" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q41" s="1"/>
-      <c r="R41" s="1">
-        <v>1</v>
-      </c>
-      <c r="S41" s="1">
-        <v>1</v>
-      </c>
-      <c r="T41" s="1">
-        <v>1</v>
-      </c>
-      <c r="U41" s="1"/>
-      <c r="V41" s="1">
-        <v>1</v>
-      </c>
-      <c r="W41" s="1"/>
-      <c r="Y41" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA41" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB41" s="1"/>
-      <c r="AC41" s="1"/>
-      <c r="AD41" s="1"/>
-    </row>
-    <row r="42" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="I41"/>
+      <c r="J41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="M41"/>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41"/>
+      <c r="P41">
+        <v>1</v>
+      </c>
+      <c r="R41">
+        <v>1</v>
+      </c>
+      <c r="S41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+      <c r="V41">
+        <v>1</v>
+      </c>
+      <c r="X41"/>
+      <c r="Y41">
+        <v>1</v>
+      </c>
+      <c r="Z41">
+        <v>1</v>
+      </c>
+      <c r="AA41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" t="s">
         <v>265</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" t="s">
         <v>88</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E42" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="1">
+      <c r="F42">
         <v>7</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" t="s">
         <v>37</v>
       </c>
-      <c r="H42" s="1">
-        <v>1</v>
-      </c>
-      <c r="L42" s="1">
-        <v>1</v>
-      </c>
-      <c r="N42" s="1">
-        <v>1</v>
-      </c>
-      <c r="P42" s="1"/>
-      <c r="Q42" s="1"/>
-      <c r="R42" s="1"/>
-      <c r="S42" s="1">
-        <v>1</v>
-      </c>
-      <c r="T42" s="1"/>
-      <c r="U42" s="1"/>
-      <c r="V42" s="1">
-        <v>1</v>
-      </c>
-      <c r="W42" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y42" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z42" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA42" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB42" s="1"/>
-      <c r="AC42" s="1"/>
-      <c r="AD42" s="1"/>
-    </row>
-    <row r="43" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42"/>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42"/>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="R42"/>
+      <c r="S42">
+        <v>1</v>
+      </c>
+      <c r="V42">
+        <v>1</v>
+      </c>
+      <c r="W42">
+        <v>1</v>
+      </c>
+      <c r="X42"/>
+      <c r="Y42">
+        <v>1</v>
+      </c>
+      <c r="Z42">
+        <v>1</v>
+      </c>
+      <c r="AA42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" t="s">
         <v>265</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E43" t="s">
         <v>46</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F43">
         <v>8</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" t="s">
         <v>27</v>
       </c>
-      <c r="H43" s="1">
-        <v>1</v>
-      </c>
-      <c r="L43" s="1">
-        <v>1</v>
-      </c>
-      <c r="N43" s="1"/>
-      <c r="P43" s="1"/>
-      <c r="Q43" s="1">
-        <v>1</v>
-      </c>
-      <c r="R43" s="1"/>
-      <c r="S43" s="1">
-        <v>1</v>
-      </c>
-      <c r="T43" s="1">
-        <v>1</v>
-      </c>
-      <c r="U43" s="1"/>
-      <c r="V43" s="1"/>
-      <c r="W43" s="1"/>
-      <c r="Y43" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA43" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB43" s="1"/>
-      <c r="AC43" s="1"/>
-      <c r="AD43" s="1"/>
-    </row>
-    <row r="44" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+      <c r="O43"/>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="R43"/>
+      <c r="S43">
+        <v>1</v>
+      </c>
+      <c r="T43">
+        <v>1</v>
+      </c>
+      <c r="X43"/>
+      <c r="Y43">
+        <v>1</v>
+      </c>
+      <c r="Z43">
+        <v>1</v>
+      </c>
+      <c r="AA43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>80</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" t="s">
         <v>81</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" t="s">
         <v>265</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" t="s">
         <v>80</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E44" t="s">
         <v>46</v>
       </c>
-      <c r="F44" s="1">
+      <c r="F44">
         <v>8</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" t="s">
         <v>27</v>
       </c>
-      <c r="H44" s="1">
-        <v>1</v>
-      </c>
-      <c r="L44" s="1">
-        <v>1</v>
-      </c>
-      <c r="N44" s="1"/>
-      <c r="P44" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1">
-        <v>1</v>
-      </c>
-      <c r="S44" s="1">
-        <v>1</v>
-      </c>
-      <c r="T44" s="1">
-        <v>1</v>
-      </c>
-      <c r="U44" s="1"/>
-      <c r="V44" s="1">
-        <v>1</v>
-      </c>
-      <c r="W44" s="1"/>
-      <c r="Y44" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA44" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB44" s="1"/>
-      <c r="AC44" s="1"/>
-      <c r="AD44" s="1"/>
-    </row>
-    <row r="45" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44"/>
+      <c r="P44">
+        <v>1</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+      <c r="T44">
+        <v>1</v>
+      </c>
+      <c r="V44">
+        <v>1</v>
+      </c>
+      <c r="X44"/>
+      <c r="Y44">
+        <v>1</v>
+      </c>
+      <c r="Z44">
+        <v>1</v>
+      </c>
+      <c r="AA44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>243</v>
       </c>
-      <c r="B45" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B45" t="s">
+        <v>279</v>
+      </c>
+      <c r="C45" t="s">
         <v>265</v>
       </c>
       <c r="F45">
@@ -4106,10 +4272,19 @@
       <c r="H45">
         <v>1</v>
       </c>
+      <c r="I45"/>
+      <c r="J45">
+        <v>1</v>
+      </c>
+      <c r="K45"/>
       <c r="L45">
         <v>1</v>
       </c>
-      <c r="N45">
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="O45"/>
+      <c r="P45">
         <v>1</v>
       </c>
       <c r="R45">
@@ -4118,11 +4293,15 @@
       <c r="S45">
         <v>1</v>
       </c>
+      <c r="V45">
+        <v>1</v>
+      </c>
+      <c r="X45"/>
       <c r="AA45">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>225</v>
       </c>
@@ -4154,7 +4333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>191</v>
       </c>
@@ -4195,7 +4374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>194</v>
       </c>
@@ -4410,7 +4589,7 @@
       <c r="N53">
         <v>1</v>
       </c>
-      <c r="R53">
+      <c r="R53" s="16">
         <v>1</v>
       </c>
       <c r="S53">
@@ -4547,7 +4726,6 @@
       </c>
       <c r="P57" s="1"/>
       <c r="Q57" s="1"/>
-      <c r="R57" s="1"/>
       <c r="S57" s="1">
         <v>1</v>
       </c>
@@ -4597,7 +4775,6 @@
       </c>
       <c r="P58" s="1"/>
       <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
       <c r="S58" s="1">
         <v>1</v>
       </c>
@@ -4683,7 +4860,6 @@
         <v>1</v>
       </c>
       <c r="Q60" s="1"/>
-      <c r="R60" s="1"/>
       <c r="S60" s="1">
         <v>1</v>
       </c>
@@ -4729,7 +4905,6 @@
       </c>
       <c r="P61" s="1"/>
       <c r="Q61" s="1"/>
-      <c r="R61" s="1"/>
       <c r="S61" s="1">
         <v>1</v>
       </c>
@@ -4775,7 +4950,6 @@
       </c>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
       <c r="S62" s="1">
         <v>1</v>
       </c>
@@ -4856,7 +5030,7 @@
       <c r="Q64" s="7">
         <v>1</v>
       </c>
-      <c r="R64" s="7">
+      <c r="R64" s="16">
         <v>1</v>
       </c>
       <c r="S64" s="7">
@@ -4904,7 +5078,7 @@
         <v>1</v>
       </c>
       <c r="Q65" s="1"/>
-      <c r="R65" s="1">
+      <c r="R65" s="16">
         <v>1</v>
       </c>
       <c r="S65" s="1">
@@ -4946,7 +5120,7 @@
       <c r="N66" s="7">
         <v>1</v>
       </c>
-      <c r="R66" s="7">
+      <c r="R66" s="16">
         <v>1</v>
       </c>
       <c r="S66" s="7">
@@ -4997,7 +5171,7 @@
       <c r="Q67" s="1">
         <v>1</v>
       </c>
-      <c r="R67" s="1">
+      <c r="R67" s="16">
         <v>1</v>
       </c>
       <c r="S67" s="1">
@@ -5055,7 +5229,7 @@
       <c r="Q68" s="1">
         <v>1</v>
       </c>
-      <c r="R68" s="1">
+      <c r="R68" s="16">
         <v>1</v>
       </c>
       <c r="S68" s="1">
@@ -5101,7 +5275,7 @@
       <c r="Q69" s="7">
         <v>1</v>
       </c>
-      <c r="R69" s="7">
+      <c r="R69" s="16">
         <v>1</v>
       </c>
       <c r="S69" s="7">
@@ -5148,7 +5322,7 @@
       <c r="Q70" s="7">
         <v>1</v>
       </c>
-      <c r="R70" s="7">
+      <c r="R70" s="16">
         <v>1</v>
       </c>
       <c r="S70" s="7">
@@ -5193,7 +5367,7 @@
       <c r="Q71" s="1">
         <v>1</v>
       </c>
-      <c r="R71" s="1">
+      <c r="R71" s="16">
         <v>1</v>
       </c>
       <c r="S71" s="1">
@@ -5247,7 +5421,7 @@
       <c r="Q72" s="1">
         <v>1</v>
       </c>
-      <c r="R72" s="1">
+      <c r="R72" s="16">
         <v>1</v>
       </c>
       <c r="S72" s="1">
@@ -5305,7 +5479,7 @@
         <v>1</v>
       </c>
       <c r="Q73" s="1"/>
-      <c r="R73" s="1">
+      <c r="R73" s="16">
         <v>1</v>
       </c>
       <c r="S73" s="1">
@@ -5363,7 +5537,7 @@
         <v>1</v>
       </c>
       <c r="Q74" s="1"/>
-      <c r="R74" s="1">
+      <c r="R74" s="16">
         <v>1</v>
       </c>
       <c r="S74" s="1">
@@ -5405,7 +5579,7 @@
       <c r="N75" s="7">
         <v>1</v>
       </c>
-      <c r="R75" s="7">
+      <c r="R75" s="16">
         <v>1</v>
       </c>
       <c r="S75" s="7">
@@ -8528,7 +8702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
addition of new categories
</commit_message>
<xml_diff>
--- a/services/services.xlsx
+++ b/services/services.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roise\Documents\Apam ciber\leaks\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99AD2FA-73C0-49FB-90AC-080A696EFCA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4233F5BA-B271-445D-B76F-F251E373D88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="280">
   <si>
     <t>Website</t>
   </si>
@@ -884,7 +884,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -947,15 +947,8 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -972,11 +965,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1035,11 +1023,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1056,10 +1043,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
@@ -1600,9 +1585,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AD76">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD76">
-    <sortCondition ref="C1:C76"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AD75">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD75">
+    <sortCondition ref="C1:C75"/>
   </sortState>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Website" dataDxfId="28"/>
@@ -1613,22 +1598,22 @@
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="min length"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="min mask"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="extra sec"/>
-    <tableColumn id="28" xr3:uid="{DBD2CD94-738E-449B-A23C-A6FB09DA0A31}" name="access username" dataCellStyle="Bad"/>
-    <tableColumn id="23" xr3:uid="{1803C7EB-1388-4025-995F-00763A49AF56}" name="access email" dataCellStyle="Bad"/>
-    <tableColumn id="22" xr3:uid="{0878A912-2CFE-44D3-8EEF-6EC62A578919}" name="access tlf" dataCellStyle="Bad"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="2fa"/>
-    <tableColumn id="26" xr3:uid="{CA81BFE9-83DF-479D-B0A3-83EFCFB4C7D2}" name="Nickname" dataCellStyle="Bad"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Name"/>
-    <tableColumn id="27" xr3:uid="{02F2CE9F-3AA5-4646-98D5-CB066ED14A49}" name="Surname" dataCellStyle="Bad"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="birth date"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="gender"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Profile photo" dataCellStyle="Bad"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="email"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="tlf"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="nacionality"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="location"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="address"/>
-    <tableColumn id="31" xr3:uid="{A4C60F27-3AAD-4532-9C2F-457D561542A0}" name="Photos" dataCellStyle="Bad"/>
+    <tableColumn id="28" xr3:uid="{DBD2CD94-738E-449B-A23C-A6FB09DA0A31}" name="access username" dataCellStyle="Normal"/>
+    <tableColumn id="23" xr3:uid="{1803C7EB-1388-4025-995F-00763A49AF56}" name="access email" dataCellStyle="Normal"/>
+    <tableColumn id="22" xr3:uid="{0878A912-2CFE-44D3-8EEF-6EC62A578919}" name="access tlf" dataCellStyle="Normal"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="2fa" dataCellStyle="Normal"/>
+    <tableColumn id="26" xr3:uid="{CA81BFE9-83DF-479D-B0A3-83EFCFB4C7D2}" name="Nickname" dataCellStyle="Normal"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Name" dataCellStyle="Normal"/>
+    <tableColumn id="27" xr3:uid="{02F2CE9F-3AA5-4646-98D5-CB066ED14A49}" name="Surname" dataCellStyle="Normal"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="birth date" dataCellStyle="Normal"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="gender" dataCellStyle="Normal"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Profile photo" dataCellStyle="Normal"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="email" dataCellStyle="Normal"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="tlf" dataCellStyle="Normal"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="nacionality" dataCellStyle="Normal"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="location" dataCellStyle="Normal"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="address" dataCellStyle="Normal"/>
+    <tableColumn id="31" xr3:uid="{A4C60F27-3AAD-4532-9C2F-457D561542A0}" name="Photos" dataCellStyle="Normal"/>
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Messages"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="subscription"/>
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="purchases"/>
@@ -1909,13 +1894,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD989"/>
+  <dimension ref="A1:AD988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A45" sqref="A45:XFD45"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1927,20 +1912,12 @@
     <col min="5" max="5" width="2.28515625" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
-    <col min="9" max="11" width="10.28515625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="16" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" customWidth="1"/>
-    <col min="15" max="15" width="8.85546875" style="16" customWidth="1"/>
+    <col min="8" max="11" width="10.28515625" customWidth="1"/>
+    <col min="12" max="15" width="8.85546875" customWidth="1"/>
     <col min="16" max="16" width="11.140625" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" style="16" customWidth="1"/>
-    <col min="19" max="21" width="8.85546875" customWidth="1"/>
+    <col min="17" max="21" width="8.85546875" customWidth="1"/>
     <col min="22" max="22" width="9.7109375" customWidth="1"/>
-    <col min="23" max="23" width="9.28515625" customWidth="1"/>
-    <col min="24" max="24" width="9.28515625" style="16" customWidth="1"/>
-    <col min="25" max="25" width="9.28515625" customWidth="1"/>
+    <col min="23" max="25" width="9.28515625" customWidth="1"/>
     <col min="26" max="26" width="13.28515625" customWidth="1"/>
     <col min="27" max="27" width="11.7109375" customWidth="1"/>
     <col min="28" max="29" width="8.5703125" customWidth="1"/>
@@ -1973,52 +1950,52 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" t="s">
         <v>275</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" t="s">
         <v>276</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" t="s">
         <v>277</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" t="s">
         <v>269</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>270</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" t="s">
         <v>271</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="R1" t="s">
         <v>273</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="16" t="s">
+      <c r="X1" t="s">
         <v>274</v>
       </c>
       <c r="Y1" s="1" t="s">
@@ -2064,23 +2041,18 @@
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="J2"/>
-      <c r="K2"/>
       <c r="M2">
         <v>1</v>
       </c>
-      <c r="O2"/>
       <c r="Q2">
         <v>1</v>
       </c>
-      <c r="R2"/>
       <c r="S2">
         <v>1</v>
       </c>
       <c r="V2">
         <v>1</v>
       </c>
-      <c r="X2"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1">
         <v>1</v>
@@ -2119,16 +2091,12 @@
       <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3"/>
       <c r="J3">
         <v>1</v>
       </c>
-      <c r="K3"/>
-      <c r="M3"/>
       <c r="N3">
         <v>1</v>
       </c>
-      <c r="O3"/>
       <c r="P3">
         <v>1</v>
       </c>
@@ -2141,7 +2109,6 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="X3"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
@@ -2178,21 +2145,18 @@
       <c r="J4">
         <v>1</v>
       </c>
-      <c r="K4"/>
       <c r="L4">
         <v>1</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
-      <c r="O4"/>
       <c r="R4">
         <v>1</v>
       </c>
       <c r="S4">
         <v>1</v>
       </c>
-      <c r="X4"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1">
         <v>1</v>
@@ -2234,11 +2198,9 @@
       <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5"/>
       <c r="M5">
         <v>1</v>
       </c>
-      <c r="O5"/>
       <c r="P5">
         <v>1</v>
       </c>
@@ -2289,14 +2251,12 @@
       <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6"/>
       <c r="L6">
         <v>1</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
-      <c r="O6"/>
       <c r="P6">
         <v>1</v>
       </c>
@@ -2309,7 +2269,6 @@
       <c r="S6">
         <v>1</v>
       </c>
-      <c r="X6"/>
       <c r="Z6">
         <v>1</v>
       </c>
@@ -2333,15 +2292,12 @@
       <c r="G7" t="s">
         <v>56</v>
       </c>
-      <c r="I7"/>
       <c r="J7">
         <v>1</v>
       </c>
-      <c r="K7"/>
       <c r="L7">
         <v>1</v>
       </c>
-      <c r="M7"/>
       <c r="N7">
         <v>1</v>
       </c>
@@ -2369,7 +2325,6 @@
       <c r="W7">
         <v>1</v>
       </c>
-      <c r="X7"/>
       <c r="Y7">
         <v>1</v>
       </c>
@@ -2393,18 +2348,12 @@
       <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="I8"/>
       <c r="J8">
         <v>1</v>
       </c>
-      <c r="K8"/>
-      <c r="M8"/>
-      <c r="O8"/>
-      <c r="R8"/>
       <c r="S8">
         <v>1</v>
       </c>
-      <c r="X8"/>
       <c r="AB8">
         <v>1</v>
       </c>
@@ -2425,23 +2374,18 @@
       <c r="G9" t="s">
         <v>27</v>
       </c>
-      <c r="I9"/>
       <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9"/>
-      <c r="M9"/>
       <c r="N9">
         <v>1</v>
       </c>
-      <c r="O9"/>
       <c r="P9">
         <v>1</v>
       </c>
       <c r="Q9">
         <v>1</v>
       </c>
-      <c r="R9"/>
       <c r="S9">
         <v>1</v>
       </c>
@@ -2451,7 +2395,6 @@
       <c r="W9">
         <v>1</v>
       </c>
-      <c r="X9"/>
       <c r="AB9">
         <v>1</v>
       </c>
@@ -2472,26 +2415,21 @@
       <c r="G10" t="s">
         <v>101</v>
       </c>
-      <c r="I10"/>
       <c r="J10">
         <v>1</v>
       </c>
-      <c r="K10"/>
       <c r="L10">
         <v>1</v>
       </c>
-      <c r="M10"/>
       <c r="N10">
         <v>1</v>
       </c>
-      <c r="O10"/>
       <c r="R10">
         <v>1</v>
       </c>
       <c r="S10">
         <v>1</v>
       </c>
-      <c r="X10"/>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -2509,26 +2447,21 @@
       <c r="G11" t="s">
         <v>27</v>
       </c>
-      <c r="I11"/>
       <c r="J11">
         <v>1</v>
       </c>
-      <c r="K11"/>
       <c r="L11">
         <v>1</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
-      <c r="O11"/>
-      <c r="R11"/>
       <c r="S11">
         <v>1</v>
       </c>
       <c r="V11">
         <v>1</v>
       </c>
-      <c r="X11"/>
       <c r="AA11">
         <v>1</v>
       </c>
@@ -2549,15 +2482,12 @@
       <c r="G12" t="s">
         <v>27</v>
       </c>
-      <c r="I12"/>
       <c r="J12">
         <v>1</v>
       </c>
-      <c r="K12"/>
       <c r="L12">
         <v>1</v>
       </c>
-      <c r="M12"/>
       <c r="N12">
         <v>1</v>
       </c>
@@ -2579,7 +2509,6 @@
       <c r="T12">
         <v>1</v>
       </c>
-      <c r="X12"/>
       <c r="Z12">
         <v>1</v>
       </c>
@@ -2600,19 +2529,15 @@
       <c r="G13" t="s">
         <v>153</v>
       </c>
-      <c r="I13"/>
       <c r="J13">
         <v>1</v>
       </c>
-      <c r="K13"/>
-      <c r="M13"/>
       <c r="N13">
         <v>1</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
-      <c r="R13"/>
       <c r="S13">
         <v>1</v>
       </c>
@@ -2622,7 +2547,6 @@
       <c r="W13">
         <v>1</v>
       </c>
-      <c r="X13"/>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2646,8 +2570,6 @@
       <c r="I14">
         <v>1</v>
       </c>
-      <c r="J14"/>
-      <c r="K14"/>
       <c r="L14">
         <v>1</v>
       </c>
@@ -2663,7 +2585,6 @@
       <c r="Q14">
         <v>1</v>
       </c>
-      <c r="R14"/>
       <c r="S14">
         <v>1</v>
       </c>
@@ -2673,7 +2594,6 @@
       <c r="W14">
         <v>1</v>
       </c>
-      <c r="X14"/>
       <c r="AA14">
         <v>1</v>
       </c>
@@ -2694,11 +2614,9 @@
       <c r="G15" t="s">
         <v>101</v>
       </c>
-      <c r="I15"/>
       <c r="J15">
         <v>1</v>
       </c>
-      <c r="K15"/>
       <c r="L15">
         <v>1</v>
       </c>
@@ -2726,7 +2644,6 @@
       <c r="W15">
         <v>1</v>
       </c>
-      <c r="X15"/>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2747,25 +2664,21 @@
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16"/>
       <c r="J16">
         <v>1</v>
       </c>
-      <c r="K16"/>
       <c r="L16">
         <v>1</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
-      <c r="O16"/>
       <c r="R16">
         <v>1</v>
       </c>
       <c r="S16">
         <v>1</v>
       </c>
-      <c r="X16"/>
       <c r="Z16">
         <v>1</v>
       </c>
@@ -2792,15 +2705,12 @@
       <c r="G17" t="s">
         <v>27</v>
       </c>
-      <c r="I17"/>
       <c r="J17">
         <v>1</v>
       </c>
-      <c r="K17"/>
       <c r="L17">
         <v>1</v>
       </c>
-      <c r="M17"/>
       <c r="N17">
         <v>1</v>
       </c>
@@ -2813,7 +2723,6 @@
       <c r="S17">
         <v>1</v>
       </c>
-      <c r="X17"/>
       <c r="Z17">
         <v>1</v>
       </c>
@@ -2834,15 +2743,12 @@
       <c r="G18" t="s">
         <v>56</v>
       </c>
-      <c r="I18"/>
       <c r="J18">
         <v>1</v>
       </c>
-      <c r="K18"/>
       <c r="L18">
         <v>1</v>
       </c>
-      <c r="M18"/>
       <c r="N18">
         <v>1</v>
       </c>
@@ -2855,7 +2761,6 @@
       <c r="S18">
         <v>1</v>
       </c>
-      <c r="X18"/>
       <c r="Z18">
         <v>1</v>
       </c>
@@ -2879,15 +2784,12 @@
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19"/>
       <c r="J19">
         <v>1</v>
       </c>
-      <c r="K19"/>
       <c r="L19">
         <v>1</v>
       </c>
-      <c r="M19"/>
       <c r="N19">
         <v>1</v>
       </c>
@@ -2909,7 +2811,6 @@
       <c r="U19">
         <v>1</v>
       </c>
-      <c r="X19"/>
       <c r="Z19">
         <v>1</v>
       </c>
@@ -2930,29 +2831,24 @@
       <c r="G20" t="s">
         <v>27</v>
       </c>
-      <c r="I20"/>
       <c r="J20">
         <v>1</v>
       </c>
-      <c r="K20"/>
       <c r="L20">
         <v>1</v>
       </c>
-      <c r="M20"/>
       <c r="N20">
         <v>1</v>
       </c>
       <c r="O20">
         <v>1</v>
       </c>
-      <c r="R20"/>
       <c r="S20">
         <v>1</v>
       </c>
       <c r="V20">
         <v>1</v>
       </c>
-      <c r="X20"/>
       <c r="Z20">
         <v>1</v>
       </c>
@@ -2982,19 +2878,15 @@
       <c r="J21">
         <v>1</v>
       </c>
-      <c r="K21"/>
       <c r="M21">
         <v>1</v>
       </c>
       <c r="N21">
         <v>1</v>
       </c>
-      <c r="O21"/>
-      <c r="R21"/>
       <c r="S21">
         <v>1</v>
       </c>
-      <c r="X21"/>
       <c r="Z21">
         <v>1</v>
       </c>
@@ -3015,18 +2907,12 @@
       <c r="G22" t="s">
         <v>101</v>
       </c>
-      <c r="I22"/>
       <c r="J22">
         <v>1</v>
       </c>
-      <c r="K22"/>
-      <c r="M22"/>
-      <c r="O22"/>
-      <c r="R22"/>
       <c r="S22">
         <v>1</v>
       </c>
-      <c r="X22"/>
       <c r="AA22">
         <v>1</v>
       </c>
@@ -3047,15 +2933,12 @@
       <c r="G23" t="s">
         <v>101</v>
       </c>
-      <c r="I23"/>
       <c r="J23">
         <v>1</v>
       </c>
-      <c r="K23"/>
       <c r="L23">
         <v>1</v>
       </c>
-      <c r="M23"/>
       <c r="N23">
         <v>1</v>
       </c>
@@ -3068,7 +2951,6 @@
       <c r="S23">
         <v>1</v>
       </c>
-      <c r="X23"/>
       <c r="Z23">
         <v>1</v>
       </c>
@@ -3089,29 +2971,24 @@
       <c r="G24" t="s">
         <v>27</v>
       </c>
-      <c r="I24"/>
       <c r="J24">
         <v>1</v>
       </c>
-      <c r="K24"/>
       <c r="M24">
         <v>1</v>
       </c>
-      <c r="O24"/>
       <c r="P24">
         <v>1</v>
       </c>
       <c r="Q24">
         <v>1</v>
       </c>
-      <c r="R24"/>
       <c r="S24">
         <v>1</v>
       </c>
       <c r="U24">
         <v>1</v>
       </c>
-      <c r="X24"/>
     </row>
     <row r="25" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -3135,15 +3012,12 @@
       <c r="G25" t="s">
         <v>33</v>
       </c>
-      <c r="I25"/>
       <c r="J25">
         <v>1</v>
       </c>
-      <c r="K25"/>
       <c r="L25">
         <v>1</v>
       </c>
-      <c r="M25"/>
       <c r="N25">
         <v>1</v>
       </c>
@@ -3168,7 +3042,6 @@
       <c r="V25">
         <v>1</v>
       </c>
-      <c r="X25"/>
       <c r="Y25">
         <v>1</v>
       </c>
@@ -3201,15 +3074,12 @@
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26"/>
       <c r="J26">
         <v>1</v>
       </c>
-      <c r="K26"/>
       <c r="L26">
         <v>1</v>
       </c>
-      <c r="M26"/>
       <c r="N26">
         <v>1</v>
       </c>
@@ -3222,7 +3092,6 @@
       <c r="Q26">
         <v>1</v>
       </c>
-      <c r="R26"/>
       <c r="S26">
         <v>1</v>
       </c>
@@ -3232,7 +3101,6 @@
       <c r="W26">
         <v>1</v>
       </c>
-      <c r="X26"/>
       <c r="Y26">
         <v>1</v>
       </c>
@@ -3268,15 +3136,12 @@
       <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27"/>
       <c r="J27">
         <v>1</v>
       </c>
-      <c r="K27"/>
       <c r="L27">
         <v>1</v>
       </c>
-      <c r="M27"/>
       <c r="N27">
         <v>1</v>
       </c>
@@ -3298,7 +3163,6 @@
       <c r="V27">
         <v>1</v>
       </c>
-      <c r="X27"/>
       <c r="Y27">
         <v>1</v>
       </c>
@@ -3337,15 +3201,12 @@
       <c r="H28">
         <v>1</v>
       </c>
-      <c r="I28"/>
       <c r="J28">
         <v>1</v>
       </c>
-      <c r="K28"/>
       <c r="L28">
         <v>1</v>
       </c>
-      <c r="M28"/>
       <c r="N28">
         <v>1</v>
       </c>
@@ -3358,14 +3219,12 @@
       <c r="Q28">
         <v>1</v>
       </c>
-      <c r="R28"/>
       <c r="S28">
         <v>1</v>
       </c>
       <c r="T28">
         <v>1</v>
       </c>
-      <c r="X28"/>
       <c r="Y28">
         <v>1</v>
       </c>
@@ -3398,29 +3257,24 @@
       <c r="H29">
         <v>1</v>
       </c>
-      <c r="I29"/>
       <c r="J29">
         <v>1</v>
       </c>
-      <c r="K29"/>
       <c r="L29">
         <v>1</v>
       </c>
-      <c r="M29"/>
       <c r="N29">
         <v>1</v>
       </c>
       <c r="O29">
         <v>1</v>
       </c>
-      <c r="R29"/>
       <c r="S29">
         <v>1</v>
       </c>
       <c r="T29">
         <v>1</v>
       </c>
-      <c r="X29"/>
       <c r="Y29">
         <v>1</v>
       </c>
@@ -3444,22 +3298,18 @@
       <c r="G30" t="s">
         <v>69</v>
       </c>
-      <c r="I30"/>
       <c r="J30">
         <v>1</v>
       </c>
-      <c r="K30"/>
       <c r="M30">
         <v>1</v>
       </c>
-      <c r="O30"/>
       <c r="R30">
         <v>1</v>
       </c>
       <c r="S30">
         <v>1</v>
       </c>
-      <c r="X30"/>
     </row>
     <row r="31" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -3486,20 +3336,15 @@
       <c r="H31">
         <v>1</v>
       </c>
-      <c r="I31"/>
       <c r="J31">
         <v>1</v>
       </c>
-      <c r="K31"/>
       <c r="M31">
         <v>1</v>
       </c>
-      <c r="O31"/>
-      <c r="R31"/>
       <c r="S31">
         <v>1</v>
       </c>
-      <c r="X31"/>
       <c r="Z31">
         <v>1</v>
       </c>
@@ -3526,23 +3371,18 @@
       <c r="G32" t="s">
         <v>27</v>
       </c>
-      <c r="I32"/>
       <c r="J32">
         <v>1</v>
       </c>
-      <c r="K32"/>
       <c r="M32">
         <v>1</v>
       </c>
-      <c r="O32"/>
-      <c r="R32"/>
       <c r="S32">
         <v>1</v>
       </c>
       <c r="T32">
         <v>1</v>
       </c>
-      <c r="X32"/>
       <c r="Z32">
         <v>1</v>
       </c>
@@ -3569,15 +3409,12 @@
       <c r="G33" t="s">
         <v>37</v>
       </c>
-      <c r="I33"/>
       <c r="J33">
         <v>1</v>
       </c>
-      <c r="K33"/>
       <c r="M33">
         <v>1</v>
       </c>
-      <c r="O33"/>
       <c r="P33">
         <v>1</v>
       </c>
@@ -3596,7 +3433,6 @@
       <c r="W33">
         <v>1</v>
       </c>
-      <c r="X33"/>
       <c r="Z33">
         <v>1</v>
       </c>
@@ -3626,15 +3462,12 @@
       <c r="I34">
         <v>1</v>
       </c>
-      <c r="J34"/>
-      <c r="K34"/>
       <c r="L34">
         <v>1</v>
       </c>
       <c r="M34">
         <v>1</v>
       </c>
-      <c r="O34"/>
       <c r="P34">
         <v>1</v>
       </c>
@@ -3647,7 +3480,6 @@
       <c r="T34">
         <v>1</v>
       </c>
-      <c r="X34"/>
       <c r="Y34">
         <v>1</v>
       </c>
@@ -3680,12 +3512,9 @@
       <c r="I35">
         <v>1</v>
       </c>
-      <c r="J35"/>
-      <c r="K35"/>
       <c r="L35">
         <v>1</v>
       </c>
-      <c r="M35"/>
       <c r="N35">
         <v>1</v>
       </c>
@@ -3695,7 +3524,6 @@
       <c r="P35">
         <v>1</v>
       </c>
-      <c r="R35"/>
       <c r="S35">
         <v>1</v>
       </c>
@@ -3705,7 +3533,6 @@
       <c r="W35">
         <v>1</v>
       </c>
-      <c r="X35"/>
       <c r="AA35">
         <v>1</v>
       </c>
@@ -3741,12 +3568,9 @@
       <c r="I36">
         <v>1</v>
       </c>
-      <c r="J36"/>
-      <c r="K36"/>
       <c r="L36">
         <v>1</v>
       </c>
-      <c r="M36"/>
       <c r="N36">
         <v>1</v>
       </c>
@@ -3756,7 +3580,6 @@
       <c r="P36">
         <v>1</v>
       </c>
-      <c r="R36"/>
       <c r="S36">
         <v>1</v>
       </c>
@@ -3769,7 +3592,6 @@
       <c r="W36">
         <v>1</v>
       </c>
-      <c r="X36"/>
       <c r="AA36">
         <v>1</v>
       </c>
@@ -3796,7 +3618,6 @@
       <c r="H37">
         <v>1</v>
       </c>
-      <c r="I37"/>
       <c r="J37">
         <v>1</v>
       </c>
@@ -3806,7 +3627,6 @@
       <c r="L37">
         <v>1</v>
       </c>
-      <c r="M37"/>
       <c r="N37">
         <v>1</v>
       </c>
@@ -3831,7 +3651,6 @@
       <c r="W37">
         <v>1</v>
       </c>
-      <c r="X37"/>
       <c r="AA37">
         <v>1</v>
       </c>
@@ -3864,7 +3683,6 @@
       <c r="J38">
         <v>1</v>
       </c>
-      <c r="K38"/>
       <c r="L38">
         <v>1</v>
       </c>
@@ -3877,14 +3695,12 @@
       <c r="O38">
         <v>1</v>
       </c>
-      <c r="R38"/>
       <c r="S38">
         <v>1</v>
       </c>
       <c r="T38">
         <v>1</v>
       </c>
-      <c r="X38"/>
       <c r="Z38">
         <v>1</v>
       </c>
@@ -3914,12 +3730,9 @@
       <c r="I39">
         <v>1</v>
       </c>
-      <c r="J39"/>
-      <c r="K39"/>
       <c r="L39">
         <v>1</v>
       </c>
-      <c r="M39"/>
       <c r="N39">
         <v>1</v>
       </c>
@@ -3929,7 +3742,6 @@
       <c r="P39">
         <v>1</v>
       </c>
-      <c r="R39"/>
       <c r="S39">
         <v>1</v>
       </c>
@@ -3939,7 +3751,6 @@
       <c r="W39">
         <v>1</v>
       </c>
-      <c r="X39"/>
       <c r="AA39">
         <v>1</v>
       </c>
@@ -3975,7 +3786,6 @@
       <c r="J40">
         <v>1</v>
       </c>
-      <c r="K40"/>
       <c r="M40">
         <v>1</v>
       </c>
@@ -3994,7 +3804,6 @@
       <c r="V40">
         <v>1</v>
       </c>
-      <c r="X40"/>
       <c r="Y40">
         <v>1</v>
       </c>
@@ -4024,18 +3833,15 @@
       <c r="G41" t="s">
         <v>56</v>
       </c>
-      <c r="I41"/>
       <c r="J41">
         <v>1</v>
       </c>
       <c r="K41">
         <v>1</v>
       </c>
-      <c r="M41"/>
       <c r="N41">
         <v>1</v>
       </c>
-      <c r="O41"/>
       <c r="P41">
         <v>1</v>
       </c>
@@ -4051,7 +3857,6 @@
       <c r="V41">
         <v>1</v>
       </c>
-      <c r="X41"/>
       <c r="Y41">
         <v>1</v>
       </c>
@@ -4087,11 +3892,9 @@
       <c r="H42">
         <v>1</v>
       </c>
-      <c r="I42"/>
       <c r="J42">
         <v>1</v>
       </c>
-      <c r="K42"/>
       <c r="L42">
         <v>1</v>
       </c>
@@ -4104,7 +3907,6 @@
       <c r="O42">
         <v>1</v>
       </c>
-      <c r="R42"/>
       <c r="S42">
         <v>1</v>
       </c>
@@ -4114,7 +3916,6 @@
       <c r="W42">
         <v>1</v>
       </c>
-      <c r="X42"/>
       <c r="Y42">
         <v>1</v>
       </c>
@@ -4165,18 +3966,15 @@
       <c r="M43">
         <v>1</v>
       </c>
-      <c r="O43"/>
       <c r="Q43">
         <v>1</v>
       </c>
-      <c r="R43"/>
       <c r="S43">
         <v>1</v>
       </c>
       <c r="T43">
         <v>1</v>
       </c>
-      <c r="X43"/>
       <c r="Y43">
         <v>1</v>
       </c>
@@ -4215,8 +4013,6 @@
       <c r="I44">
         <v>1</v>
       </c>
-      <c r="J44"/>
-      <c r="K44"/>
       <c r="L44">
         <v>1</v>
       </c>
@@ -4226,7 +4022,6 @@
       <c r="N44">
         <v>1</v>
       </c>
-      <c r="O44"/>
       <c r="P44">
         <v>1</v>
       </c>
@@ -4242,7 +4037,6 @@
       <c r="V44">
         <v>1</v>
       </c>
-      <c r="X44"/>
       <c r="Y44">
         <v>1</v>
       </c>
@@ -4272,18 +4066,15 @@
       <c r="H45">
         <v>1</v>
       </c>
-      <c r="I45"/>
       <c r="J45">
         <v>1</v>
       </c>
-      <c r="K45"/>
       <c r="L45">
         <v>1</v>
       </c>
       <c r="M45">
         <v>1</v>
       </c>
-      <c r="O45"/>
       <c r="P45">
         <v>1</v>
       </c>
@@ -4296,19 +4087,18 @@
       <c r="V45">
         <v>1</v>
       </c>
-      <c r="X45"/>
       <c r="AA45">
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="A46" t="s">
         <v>225</v>
       </c>
       <c r="B46" t="s">
         <v>233</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C46" t="s">
         <v>265</v>
       </c>
       <c r="F46">
@@ -4317,9 +4107,15 @@
       <c r="G46" t="s">
         <v>27</v>
       </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
       <c r="N46">
         <v>1</v>
       </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
       <c r="Q46">
         <v>1</v>
       </c>
@@ -4334,7 +4130,7 @@
       </c>
     </row>
     <row r="47" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" t="s">
         <v>191</v>
       </c>
       <c r="B47" t="s">
@@ -4355,12 +4151,24 @@
       <c r="G47" t="s">
         <v>101</v>
       </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
       <c r="L47">
         <v>1</v>
       </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
       <c r="N47">
         <v>1</v>
       </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
       <c r="S47">
         <v>1</v>
       </c>
@@ -4375,7 +4183,7 @@
       </c>
     </row>
     <row r="48" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="A48" t="s">
         <v>194</v>
       </c>
       <c r="B48" t="s">
@@ -4393,12 +4201,24 @@
       <c r="G48" t="s">
         <v>27</v>
       </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>1</v>
+      </c>
       <c r="L48">
         <v>1</v>
       </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
       <c r="N48">
         <v>1</v>
       </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
       <c r="S48">
         <v>1</v>
       </c>
@@ -4412,8 +4232,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+    <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>199</v>
       </c>
       <c r="B49" t="s">
@@ -4431,12 +4251,18 @@
       <c r="H49">
         <v>1</v>
       </c>
+      <c r="J49">
+        <v>1</v>
+      </c>
       <c r="L49">
         <v>1</v>
       </c>
       <c r="N49">
         <v>1</v>
       </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
       <c r="S49">
         <v>1</v>
       </c>
@@ -4450,8 +4276,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>201</v>
       </c>
       <c r="B50" t="s">
@@ -4469,12 +4295,21 @@
       <c r="H50">
         <v>1</v>
       </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
       <c r="L50">
         <v>1</v>
       </c>
       <c r="N50">
         <v>1</v>
       </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
       <c r="S50">
         <v>1</v>
       </c>
@@ -4491,8 +4326,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+    <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>197</v>
       </c>
       <c r="B51" t="s">
@@ -4507,12 +4342,21 @@
       <c r="G51" t="s">
         <v>27</v>
       </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
       <c r="L51">
         <v>1</v>
       </c>
       <c r="N51">
         <v>1</v>
       </c>
+      <c r="O51">
+        <v>1</v>
+      </c>
+      <c r="R51">
+        <v>1</v>
+      </c>
       <c r="S51">
         <v>1</v>
       </c>
@@ -4526,14 +4370,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>250</v>
       </c>
       <c r="B52" t="s">
         <v>251</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="C52" t="s">
         <v>247</v>
       </c>
       <c r="F52">
@@ -4542,18 +4386,27 @@
       <c r="G52" t="s">
         <v>27</v>
       </c>
+      <c r="J52">
+        <v>1</v>
+      </c>
       <c r="L52">
         <v>1</v>
       </c>
       <c r="N52">
         <v>1</v>
       </c>
+      <c r="O52">
+        <v>1</v>
+      </c>
       <c r="P52">
         <v>1</v>
       </c>
       <c r="Q52">
         <v>1</v>
       </c>
+      <c r="R52">
+        <v>1</v>
+      </c>
       <c r="S52">
         <v>1</v>
       </c>
@@ -4567,14 +4420,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>252</v>
       </c>
       <c r="B53" t="s">
         <v>253</v>
       </c>
-      <c r="C53" s="1" t="s">
+      <c r="C53" t="s">
         <v>247</v>
       </c>
       <c r="F53">
@@ -4586,10 +4439,13 @@
       <c r="H53">
         <v>1</v>
       </c>
-      <c r="N53">
-        <v>1</v>
-      </c>
-      <c r="R53" s="16">
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="R53">
         <v>1</v>
       </c>
       <c r="S53">
@@ -4608,14 +4464,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>248</v>
       </c>
       <c r="B54" t="s">
         <v>249</v>
       </c>
-      <c r="C54" s="1" t="s">
+      <c r="C54" t="s">
         <v>247</v>
       </c>
       <c r="F54">
@@ -4624,9 +4480,21 @@
       <c r="G54" t="s">
         <v>37</v>
       </c>
+      <c r="J54">
+        <v>1</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
       <c r="N54">
         <v>1</v>
       </c>
+      <c r="O54">
+        <v>1</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
       <c r="S54">
         <v>1</v>
       </c>
@@ -4634,14 +4502,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>181</v>
       </c>
       <c r="B55" t="s">
         <v>182</v>
       </c>
-      <c r="C55" s="1" t="s">
+      <c r="C55" t="s">
         <v>247</v>
       </c>
       <c r="E55" t="s">
@@ -4653,7 +4521,10 @@
       <c r="G55" t="s">
         <v>37</v>
       </c>
-      <c r="N55">
+      <c r="J55">
+        <v>1</v>
+      </c>
+      <c r="M55">
         <v>1</v>
       </c>
       <c r="P55">
@@ -4666,14 +4537,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+    <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>179</v>
       </c>
       <c r="B56" t="s">
         <v>180</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="C56" t="s">
         <v>247</v>
       </c>
       <c r="E56" t="s">
@@ -4685,292 +4556,287 @@
       <c r="G56" t="s">
         <v>27</v>
       </c>
+      <c r="J56">
+        <v>1</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
       <c r="N56">
         <v>1</v>
       </c>
+      <c r="O56">
+        <v>1</v>
+      </c>
       <c r="S56">
         <v>1</v>
       </c>
+      <c r="V56">
+        <v>1</v>
+      </c>
       <c r="Z56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+    <row r="57" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>107</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C57" t="s">
         <v>109</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" t="s">
         <v>107</v>
       </c>
-      <c r="E57" s="1" t="s">
+      <c r="E57" t="s">
         <v>46</v>
       </c>
-      <c r="F57" s="1">
+      <c r="F57">
         <v>6</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="G57" t="s">
         <v>27</v>
       </c>
-      <c r="H57" s="1"/>
-      <c r="L57" s="1">
-        <v>1</v>
-      </c>
-      <c r="N57" s="1">
-        <v>1</v>
-      </c>
-      <c r="P57" s="1"/>
-      <c r="Q57" s="1"/>
-      <c r="S57" s="1">
-        <v>1</v>
-      </c>
-      <c r="T57" s="1">
-        <v>1</v>
-      </c>
-      <c r="U57" s="1"/>
-      <c r="V57" s="1"/>
-      <c r="W57" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y57" s="1"/>
-      <c r="Z57" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA57" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB57" s="1"/>
-      <c r="AC57" s="1"/>
-      <c r="AD57" s="1"/>
-    </row>
-    <row r="58" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="J57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>1</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="S57">
+        <v>1</v>
+      </c>
+      <c r="T57">
+        <v>1</v>
+      </c>
+      <c r="W57">
+        <v>1</v>
+      </c>
+      <c r="Z57">
+        <v>1</v>
+      </c>
+      <c r="AA57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>141</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" t="s">
         <v>142</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" t="s">
         <v>109</v>
       </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1">
+      <c r="F58">
         <v>6</v>
       </c>
-      <c r="G58" s="1" t="s">
+      <c r="G58" t="s">
         <v>27</v>
       </c>
-      <c r="H58" s="1"/>
-      <c r="L58" s="1">
-        <v>1</v>
-      </c>
-      <c r="N58" s="1">
-        <v>1</v>
-      </c>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="S58" s="1">
-        <v>1</v>
-      </c>
-      <c r="T58" s="1"/>
-      <c r="U58" s="1"/>
-      <c r="V58" s="1">
-        <v>1</v>
-      </c>
-      <c r="W58" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y58" s="1"/>
-      <c r="Z58" s="1"/>
-      <c r="AA58" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB58" s="1"/>
-      <c r="AC58" s="1"/>
-      <c r="AD58" s="1"/>
-    </row>
-    <row r="59" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>1</v>
+      </c>
+      <c r="N58">
+        <v>1</v>
+      </c>
+      <c r="S58">
+        <v>1</v>
+      </c>
+      <c r="V58">
+        <v>1</v>
+      </c>
+      <c r="W58">
+        <v>1</v>
+      </c>
+      <c r="AA58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>211</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="B59" t="s">
         <v>212</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" t="s">
         <v>109</v>
       </c>
       <c r="F59">
         <v>8</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="G59" t="s">
         <v>56</v>
       </c>
-      <c r="N59" s="7">
-        <v>1</v>
-      </c>
-      <c r="S59" s="7">
-        <v>1</v>
-      </c>
-      <c r="T59" s="7">
-        <v>1</v>
-      </c>
-      <c r="W59" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA59" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="J59">
+        <v>1</v>
+      </c>
+      <c r="N59">
+        <v>1</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+      <c r="S59">
+        <v>1</v>
+      </c>
+      <c r="T59">
+        <v>1</v>
+      </c>
+      <c r="W59">
+        <v>1</v>
+      </c>
+      <c r="AA59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>110</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" t="s">
         <v>109</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" t="s">
         <v>110</v>
       </c>
-      <c r="E60" s="1" t="s">
+      <c r="E60" t="s">
         <v>100</v>
       </c>
-      <c r="F60" s="1">
+      <c r="F60">
         <v>8</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="G60" t="s">
         <v>101</v>
       </c>
-      <c r="H60" s="1">
-        <v>1</v>
-      </c>
-      <c r="L60" s="1"/>
-      <c r="N60" s="1">
-        <v>1</v>
-      </c>
-      <c r="P60" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q60" s="1"/>
-      <c r="S60" s="1">
-        <v>1</v>
-      </c>
-      <c r="T60" s="1"/>
-      <c r="U60" s="1"/>
-      <c r="V60" s="1"/>
-      <c r="W60" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y60" s="1"/>
-      <c r="Z60" s="1"/>
-      <c r="AA60" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB60" s="1"/>
-      <c r="AC60" s="1"/>
-      <c r="AD60" s="1"/>
-    </row>
-    <row r="61" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="H60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>1</v>
+      </c>
+      <c r="N60">
+        <v>1</v>
+      </c>
+      <c r="O60">
+        <v>1</v>
+      </c>
+      <c r="P60">
+        <v>1</v>
+      </c>
+      <c r="S60">
+        <v>1</v>
+      </c>
+      <c r="W60">
+        <v>1</v>
+      </c>
+      <c r="AA60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>134</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" t="s">
         <v>135</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" t="s">
         <v>109</v>
       </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1">
+      <c r="F61">
         <v>8</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="G61" t="s">
         <v>27</v>
       </c>
-      <c r="H61" s="1"/>
-      <c r="L61" s="1">
-        <v>1</v>
-      </c>
-      <c r="N61" s="1">
-        <v>1</v>
-      </c>
-      <c r="P61" s="1"/>
-      <c r="Q61" s="1"/>
-      <c r="S61" s="1">
-        <v>1</v>
-      </c>
-      <c r="T61" s="1"/>
-      <c r="U61" s="1"/>
-      <c r="V61" s="1"/>
-      <c r="W61" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y61" s="1"/>
-      <c r="Z61" s="1"/>
-      <c r="AA61" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB61" s="1"/>
-      <c r="AC61" s="1"/>
-      <c r="AD61" s="1"/>
-    </row>
-    <row r="62" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>1</v>
+      </c>
+      <c r="N61">
+        <v>1</v>
+      </c>
+      <c r="R61">
+        <v>1</v>
+      </c>
+      <c r="S61">
+        <v>1</v>
+      </c>
+      <c r="W61">
+        <v>1</v>
+      </c>
+      <c r="AA61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>143</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B62" t="s">
         <v>144</v>
       </c>
-      <c r="C62" s="1" t="s">
+      <c r="C62" t="s">
         <v>109</v>
       </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1">
+      <c r="F62">
         <v>6</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="G62" t="s">
         <v>56</v>
       </c>
-      <c r="H62" s="1"/>
-      <c r="L62" s="1">
-        <v>1</v>
-      </c>
-      <c r="N62" s="1">
-        <v>1</v>
-      </c>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
-      <c r="S62" s="1">
-        <v>1</v>
-      </c>
-      <c r="T62" s="1">
-        <v>1</v>
-      </c>
-      <c r="U62" s="1"/>
-      <c r="V62" s="1"/>
-      <c r="W62" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y62" s="1"/>
-      <c r="Z62" s="1"/>
-      <c r="AA62" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB62" s="1"/>
-      <c r="AC62" s="1"/>
-      <c r="AD62" s="1"/>
-    </row>
-    <row r="63" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J62">
+        <v>1</v>
+      </c>
+      <c r="L62">
+        <v>1</v>
+      </c>
+      <c r="N62">
+        <v>1</v>
+      </c>
+      <c r="O62">
+        <v>1</v>
+      </c>
+      <c r="S62">
+        <v>1</v>
+      </c>
+      <c r="T62">
+        <v>1</v>
+      </c>
+      <c r="W62">
+        <v>1</v>
+      </c>
+      <c r="AA62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>241</v>
       </c>
@@ -4984,9 +4850,15 @@
         <v>8</v>
       </c>
       <c r="G63" t="s">
-        <v>27</v>
-      </c>
-      <c r="N63">
+        <v>37</v>
+      </c>
+      <c r="J63">
+        <v>1</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="M63">
         <v>1</v>
       </c>
       <c r="Q63">
@@ -5005,297 +4877,329 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+    <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>213</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B64" t="s">
         <v>126</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" t="s">
         <v>114</v>
       </c>
       <c r="F64">
         <v>6</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="G64" t="s">
         <v>27</v>
       </c>
-      <c r="L64" s="7">
-        <v>1</v>
-      </c>
-      <c r="N64" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q64" s="7">
-        <v>1</v>
-      </c>
-      <c r="R64" s="16">
-        <v>1</v>
-      </c>
-      <c r="S64" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y64" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z64" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="J64">
+        <v>1</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="L64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <v>1</v>
+      </c>
+      <c r="O64">
+        <v>1</v>
+      </c>
+      <c r="Q64">
+        <v>1</v>
+      </c>
+      <c r="R64">
+        <v>1</v>
+      </c>
+      <c r="S64">
+        <v>1</v>
+      </c>
+      <c r="X64">
+        <v>1</v>
+      </c>
+      <c r="Y64">
+        <v>1</v>
+      </c>
+      <c r="Z64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>129</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" t="s">
         <v>130</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C65" t="s">
         <v>114</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" t="s">
         <v>131</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="E65" t="s">
         <v>46</v>
       </c>
-      <c r="F65" s="1">
+      <c r="F65">
         <v>8</v>
       </c>
-      <c r="G65" s="1" t="s">
+      <c r="G65" t="s">
         <v>27</v>
       </c>
-      <c r="H65" s="1">
-        <v>1</v>
-      </c>
-      <c r="L65" s="1">
-        <v>1</v>
-      </c>
-      <c r="N65" s="1">
-        <v>1</v>
-      </c>
-      <c r="P65" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q65" s="1"/>
-      <c r="R65" s="16">
-        <v>1</v>
-      </c>
-      <c r="S65" s="1">
-        <v>1</v>
-      </c>
-      <c r="T65" s="1">
-        <v>1</v>
-      </c>
-      <c r="U65" s="1"/>
-      <c r="V65" s="1"/>
-      <c r="W65" s="1"/>
-      <c r="Y65" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z65" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA65" s="1"/>
-      <c r="AB65" s="1"/>
-      <c r="AC65" s="1"/>
-      <c r="AD65" s="1"/>
-    </row>
-    <row r="66" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>1</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <v>1</v>
+      </c>
+      <c r="M65">
+        <v>1</v>
+      </c>
+      <c r="P65">
+        <v>1</v>
+      </c>
+      <c r="R65">
+        <v>1</v>
+      </c>
+      <c r="S65">
+        <v>1</v>
+      </c>
+      <c r="T65">
+        <v>1</v>
+      </c>
+      <c r="Y65">
+        <v>1</v>
+      </c>
+      <c r="Z65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>209</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B66" t="s">
         <v>210</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" t="s">
         <v>114</v>
       </c>
       <c r="F66">
         <v>5</v>
       </c>
-      <c r="G66" s="7" t="s">
+      <c r="G66" t="s">
         <v>27</v>
       </c>
-      <c r="N66" s="7">
-        <v>1</v>
-      </c>
-      <c r="R66" s="16">
-        <v>1</v>
-      </c>
-      <c r="S66" s="7">
-        <v>1</v>
-      </c>
-      <c r="T66" s="7">
-        <v>1</v>
-      </c>
-      <c r="V66" s="7">
+      <c r="J66">
+        <v>1</v>
+      </c>
+      <c r="M66">
+        <v>1</v>
+      </c>
+      <c r="R66">
+        <v>1</v>
+      </c>
+      <c r="S66">
+        <v>1</v>
+      </c>
+      <c r="T66">
+        <v>1</v>
+      </c>
+      <c r="V66">
+        <v>1</v>
+      </c>
+      <c r="X66">
         <v>1</v>
       </c>
       <c r="Y66">
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+    <row r="67" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>112</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" t="s">
         <v>113</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" t="s">
         <v>114</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" t="s">
         <v>115</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" t="s">
         <v>46</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F67">
         <v>6</v>
       </c>
-      <c r="G67" s="1" t="s">
+      <c r="G67" t="s">
         <v>37</v>
       </c>
-      <c r="H67" s="1"/>
-      <c r="L67" s="1">
-        <v>1</v>
-      </c>
-      <c r="N67" s="1">
-        <v>1</v>
-      </c>
-      <c r="P67" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q67" s="1">
-        <v>1</v>
-      </c>
-      <c r="R67" s="16">
-        <v>1</v>
-      </c>
-      <c r="S67" s="1">
-        <v>1</v>
-      </c>
-      <c r="T67" s="1">
-        <v>1</v>
-      </c>
-      <c r="U67" s="1"/>
-      <c r="V67" s="1">
-        <v>1</v>
-      </c>
-      <c r="W67" s="1"/>
-      <c r="Y67" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z67" s="1"/>
-      <c r="AA67" s="1"/>
-      <c r="AB67" s="1"/>
-      <c r="AC67" s="1"/>
-      <c r="AD67" s="1"/>
-    </row>
-    <row r="68" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="J67">
+        <v>1</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>1</v>
+      </c>
+      <c r="N67">
+        <v>1</v>
+      </c>
+      <c r="O67">
+        <v>1</v>
+      </c>
+      <c r="P67">
+        <v>1</v>
+      </c>
+      <c r="Q67">
+        <v>1</v>
+      </c>
+      <c r="R67">
+        <v>1</v>
+      </c>
+      <c r="S67">
+        <v>1</v>
+      </c>
+      <c r="T67">
+        <v>1</v>
+      </c>
+      <c r="V67">
+        <v>1</v>
+      </c>
+      <c r="X67">
+        <v>1</v>
+      </c>
+      <c r="Y67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>116</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" t="s">
         <v>117</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C68" t="s">
         <v>114</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" t="s">
         <v>115</v>
       </c>
-      <c r="E68" s="1" t="s">
+      <c r="E68" t="s">
         <v>46</v>
       </c>
-      <c r="F68" s="1">
+      <c r="F68">
         <v>6</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="G68" t="s">
         <v>37</v>
       </c>
-      <c r="H68" s="1"/>
-      <c r="L68" s="1">
-        <v>1</v>
-      </c>
-      <c r="N68" s="1">
-        <v>1</v>
-      </c>
-      <c r="P68" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q68" s="1">
-        <v>1</v>
-      </c>
-      <c r="R68" s="16">
-        <v>1</v>
-      </c>
-      <c r="S68" s="1">
-        <v>1</v>
-      </c>
-      <c r="T68" s="1">
-        <v>1</v>
-      </c>
-      <c r="U68" s="1"/>
-      <c r="V68" s="1"/>
-      <c r="W68" s="1"/>
-      <c r="Y68" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z68" s="1"/>
-      <c r="AA68" s="1"/>
-      <c r="AB68" s="1"/>
-      <c r="AC68" s="1"/>
-      <c r="AD68" s="1"/>
-    </row>
-    <row r="69" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>1</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="L68">
+        <v>1</v>
+      </c>
+      <c r="M68">
+        <v>1</v>
+      </c>
+      <c r="P68">
+        <v>1</v>
+      </c>
+      <c r="Q68">
+        <v>1</v>
+      </c>
+      <c r="R68">
+        <v>1</v>
+      </c>
+      <c r="S68">
+        <v>1</v>
+      </c>
+      <c r="T68">
+        <v>1</v>
+      </c>
+      <c r="X68">
+        <v>1</v>
+      </c>
+      <c r="Y68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>214</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B69" t="s">
         <v>215</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" t="s">
         <v>114</v>
       </c>
       <c r="F69">
         <v>6</v>
       </c>
-      <c r="G69" s="7" t="s">
+      <c r="G69" t="s">
         <v>27</v>
       </c>
-      <c r="N69" s="7">
-        <v>1</v>
-      </c>
-      <c r="P69" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q69" s="7">
-        <v>1</v>
-      </c>
-      <c r="R69" s="16">
-        <v>1</v>
-      </c>
-      <c r="S69" s="7">
-        <v>1</v>
-      </c>
-      <c r="V69" s="7">
-        <v>1</v>
-      </c>
-      <c r="Y69" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z69" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="J69">
+        <v>1</v>
+      </c>
+      <c r="N69">
+        <v>1</v>
+      </c>
+      <c r="O69">
+        <v>1</v>
+      </c>
+      <c r="P69">
+        <v>1</v>
+      </c>
+      <c r="Q69">
+        <v>1</v>
+      </c>
+      <c r="R69">
+        <v>1</v>
+      </c>
+      <c r="S69">
+        <v>1</v>
+      </c>
+      <c r="V69">
+        <v>1</v>
+      </c>
+      <c r="X69">
+        <v>1</v>
+      </c>
+      <c r="Y69">
+        <v>1</v>
+      </c>
+      <c r="Z69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>224</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" t="s">
         <v>230</v>
       </c>
       <c r="C70" t="s">
@@ -5304,327 +5208,316 @@
       <c r="F70">
         <v>6</v>
       </c>
-      <c r="G70" s="7" t="s">
+      <c r="G70" t="s">
         <v>101</v>
       </c>
-      <c r="H70" s="7">
-        <v>1</v>
-      </c>
-      <c r="L70" s="7">
-        <v>1</v>
-      </c>
-      <c r="N70" s="7">
-        <v>1</v>
-      </c>
-      <c r="P70" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q70" s="7">
-        <v>1</v>
-      </c>
-      <c r="R70" s="16">
-        <v>1</v>
-      </c>
-      <c r="S70" s="7">
+      <c r="H70">
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>1</v>
+      </c>
+      <c r="M70">
+        <v>1</v>
+      </c>
+      <c r="N70">
+        <v>1</v>
+      </c>
+      <c r="O70">
+        <v>1</v>
+      </c>
+      <c r="P70">
+        <v>1</v>
+      </c>
+      <c r="Q70">
+        <v>1</v>
+      </c>
+      <c r="R70">
+        <v>1</v>
+      </c>
+      <c r="S70">
+        <v>1</v>
+      </c>
+      <c r="X70">
         <v>1</v>
       </c>
       <c r="Y70">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+    <row r="71" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>127</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" t="s">
         <v>128</v>
       </c>
-      <c r="C71" s="10" t="s">
+      <c r="C71" t="s">
         <v>114</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" t="s">
         <v>127</v>
       </c>
-      <c r="E71" s="1" t="s">
+      <c r="E71" t="s">
         <v>46</v>
       </c>
-      <c r="F71" s="1">
+      <c r="F71">
         <v>6</v>
       </c>
-      <c r="G71" s="1" t="s">
+      <c r="G71" t="s">
         <v>27</v>
       </c>
-      <c r="H71" s="1"/>
-      <c r="L71" s="1">
-        <v>1</v>
-      </c>
-      <c r="N71" s="1">
-        <v>1</v>
-      </c>
-      <c r="P71" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q71" s="1">
-        <v>1</v>
-      </c>
-      <c r="R71" s="16">
-        <v>1</v>
-      </c>
-      <c r="S71" s="1">
-        <v>1</v>
-      </c>
-      <c r="T71" s="1"/>
-      <c r="U71" s="1"/>
-      <c r="V71" s="1">
-        <v>1</v>
-      </c>
-      <c r="W71" s="1"/>
-      <c r="Y71" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z71" s="1"/>
-      <c r="AA71" s="1"/>
-      <c r="AB71" s="1"/>
-      <c r="AC71" s="1"/>
-      <c r="AD71" s="1"/>
-    </row>
-    <row r="72" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="J71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>1</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+      <c r="N71">
+        <v>1</v>
+      </c>
+      <c r="O71">
+        <v>1</v>
+      </c>
+      <c r="P71">
+        <v>1</v>
+      </c>
+      <c r="Q71">
+        <v>1</v>
+      </c>
+      <c r="R71">
+        <v>1</v>
+      </c>
+      <c r="S71">
+        <v>1</v>
+      </c>
+      <c r="V71">
+        <v>1</v>
+      </c>
+      <c r="X71">
+        <v>1</v>
+      </c>
+      <c r="Y71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>121</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C72" t="s">
         <v>114</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" t="s">
         <v>25</v>
       </c>
-      <c r="E72" s="1" t="s">
+      <c r="E72" t="s">
         <v>46</v>
       </c>
-      <c r="F72" s="1">
+      <c r="F72">
         <v>8</v>
       </c>
-      <c r="G72" s="1" t="s">
+      <c r="G72" t="s">
         <v>27</v>
       </c>
-      <c r="H72" s="1">
-        <v>1</v>
-      </c>
-      <c r="L72" s="1">
-        <v>1</v>
-      </c>
-      <c r="N72" s="1"/>
-      <c r="P72" s="1"/>
-      <c r="Q72" s="1">
-        <v>1</v>
-      </c>
-      <c r="R72" s="16">
-        <v>1</v>
-      </c>
-      <c r="S72" s="1">
-        <v>1</v>
-      </c>
-      <c r="T72" s="1">
-        <v>1</v>
-      </c>
-      <c r="U72" s="1"/>
-      <c r="V72" s="1">
-        <v>1</v>
-      </c>
-      <c r="W72" s="1"/>
-      <c r="Y72" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z72" s="1"/>
-      <c r="AA72" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB72" s="1"/>
-      <c r="AC72" s="1"/>
-      <c r="AD72" s="1"/>
-    </row>
-    <row r="73" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
+      <c r="H72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>1</v>
+      </c>
+      <c r="M72">
+        <v>1</v>
+      </c>
+      <c r="Q72">
+        <v>1</v>
+      </c>
+      <c r="R72">
+        <v>1</v>
+      </c>
+      <c r="S72">
+        <v>1</v>
+      </c>
+      <c r="T72">
+        <v>1</v>
+      </c>
+      <c r="V72">
+        <v>1</v>
+      </c>
+      <c r="X72">
+        <v>1</v>
+      </c>
+      <c r="Y72">
+        <v>1</v>
+      </c>
+      <c r="AA72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>123</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" t="s">
         <v>124</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C73" t="s">
         <v>114</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" t="s">
         <v>125</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="E73" t="s">
         <v>94</v>
       </c>
-      <c r="F73" s="1">
+      <c r="F73">
         <v>8</v>
       </c>
-      <c r="G73" s="1" t="s">
+      <c r="G73" t="s">
         <v>33</v>
       </c>
-      <c r="H73" s="1"/>
-      <c r="L73" s="1">
-        <v>1</v>
-      </c>
-      <c r="N73" s="1">
-        <v>1</v>
-      </c>
-      <c r="P73" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q73" s="1"/>
-      <c r="R73" s="16">
-        <v>1</v>
-      </c>
-      <c r="S73" s="1">
-        <v>1</v>
-      </c>
-      <c r="T73" s="1">
-        <v>1</v>
-      </c>
-      <c r="U73" s="1"/>
-      <c r="V73" s="1">
-        <v>1</v>
-      </c>
-      <c r="W73" s="1"/>
-      <c r="Y73" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z73" s="1"/>
-      <c r="AA73" s="1">
-        <v>1</v>
-      </c>
-      <c r="AB73" s="1"/>
-      <c r="AC73" s="1"/>
-      <c r="AD73" s="1"/>
-    </row>
-    <row r="74" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="M73">
+        <v>1</v>
+      </c>
+      <c r="P73">
+        <v>1</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
+      </c>
+      <c r="S73">
+        <v>1</v>
+      </c>
+      <c r="T73">
+        <v>1</v>
+      </c>
+      <c r="V73">
+        <v>1</v>
+      </c>
+      <c r="X73">
+        <v>1</v>
+      </c>
+      <c r="Y73">
+        <v>1</v>
+      </c>
+      <c r="AA73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>118</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" t="s">
         <v>119</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C74" t="s">
         <v>114</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" t="s">
         <v>120</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="E74" t="s">
         <v>46</v>
       </c>
-      <c r="F74" s="1">
+      <c r="F74">
         <v>8</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="G74" t="s">
         <v>60</v>
       </c>
-      <c r="H74" s="1"/>
-      <c r="L74" s="1">
-        <v>1</v>
-      </c>
-      <c r="N74" s="1">
-        <v>1</v>
-      </c>
-      <c r="P74" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="16">
-        <v>1</v>
-      </c>
-      <c r="S74" s="1">
-        <v>1</v>
-      </c>
-      <c r="T74" s="1">
-        <v>1</v>
-      </c>
-      <c r="U74" s="1"/>
-      <c r="V74" s="1">
-        <v>1</v>
-      </c>
-      <c r="W74" s="1"/>
-      <c r="Y74" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z74" s="1"/>
-      <c r="AA74" s="1"/>
-      <c r="AB74" s="1"/>
-      <c r="AC74" s="1"/>
-      <c r="AD74" s="1"/>
-    </row>
-    <row r="75" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>1</v>
+      </c>
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>1</v>
+      </c>
+      <c r="M74">
+        <v>1</v>
+      </c>
+      <c r="P74">
+        <v>1</v>
+      </c>
+      <c r="R74">
+        <v>1</v>
+      </c>
+      <c r="S74">
+        <v>1</v>
+      </c>
+      <c r="T74">
+        <v>1</v>
+      </c>
+      <c r="V74">
+        <v>1</v>
+      </c>
+      <c r="X74">
+        <v>1</v>
+      </c>
+      <c r="Y74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>245</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="C75" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="B75" t="s">
+        <v>263</v>
+      </c>
+      <c r="C75" t="s">
         <v>114</v>
       </c>
       <c r="F75">
-        <v>5</v>
-      </c>
-      <c r="G75" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G75" t="s">
         <v>27</v>
       </c>
-      <c r="N75" s="7">
-        <v>1</v>
-      </c>
-      <c r="R75" s="16">
-        <v>1</v>
-      </c>
-      <c r="S75" s="7">
-        <v>1</v>
-      </c>
-      <c r="T75" s="7">
-        <v>1</v>
-      </c>
-      <c r="V75" s="7">
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="M75">
+        <v>1</v>
+      </c>
+      <c r="R75">
+        <v>1</v>
+      </c>
+      <c r="S75">
+        <v>1</v>
+      </c>
+      <c r="X75">
         <v>1</v>
       </c>
       <c r="Y75">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>258</v>
-      </c>
-      <c r="B76" t="s">
-        <v>263</v>
-      </c>
-      <c r="C76" t="s">
-        <v>114</v>
-      </c>
-      <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76" t="s">
-        <v>27</v>
-      </c>
-      <c r="N76">
-        <v>1</v>
-      </c>
-      <c r="S76">
-        <v>1</v>
-      </c>
-      <c r="Y76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6533,7 +6426,6 @@
     <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -7608,8 +7500,8 @@
         <v>114</v>
       </c>
       <c r="B2">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A2)</f>
-        <v>13</v>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A2)</f>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -7617,7 +7509,7 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A3)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A3)</f>
         <v>5</v>
       </c>
     </row>
@@ -7626,7 +7518,7 @@
         <v>265</v>
       </c>
       <c r="B4">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A4)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A4)</f>
         <v>7</v>
       </c>
     </row>
@@ -7635,7 +7527,7 @@
         <v>63</v>
       </c>
       <c r="B5">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A5)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A5)</f>
         <v>5</v>
       </c>
     </row>
@@ -7644,7 +7536,7 @@
         <v>165</v>
       </c>
       <c r="B6">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A6)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A6)</f>
         <v>5</v>
       </c>
     </row>
@@ -7653,7 +7545,7 @@
         <v>49</v>
       </c>
       <c r="B7">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A7)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A7)</f>
         <v>5</v>
       </c>
     </row>
@@ -7662,7 +7554,7 @@
         <v>109</v>
       </c>
       <c r="B8">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A8)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A8)</f>
         <v>7</v>
       </c>
     </row>
@@ -7671,7 +7563,7 @@
         <v>140</v>
       </c>
       <c r="B9">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A9)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A9)</f>
         <v>5</v>
       </c>
     </row>
@@ -7680,7 +7572,7 @@
         <v>133</v>
       </c>
       <c r="B10">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A10)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A10)</f>
         <v>9</v>
       </c>
     </row>
@@ -7689,7 +7581,7 @@
         <v>44</v>
       </c>
       <c r="B11">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A11)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A11)</f>
         <v>9</v>
       </c>
     </row>
@@ -7698,7 +7590,7 @@
         <v>247</v>
       </c>
       <c r="B12">
-        <f>COUNTIF(Services!$C$2:$C$76,Count!A12)</f>
+        <f>COUNTIF(Services!$C$2:$C$75,Count!A12)</f>
         <v>5</v>
       </c>
     </row>
@@ -7709,7 +7601,7 @@
       </c>
       <c r="B13" s="1">
         <f>SUM(B2:B12)</f>
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Internet rename to network operations
</commit_message>
<xml_diff>
--- a/services/services.xlsx
+++ b/services/services.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\roise\Documents\Apam ciber\leaks\services\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757D7E5F-1007-4E95-AD59-F3AF8BC134B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43721DD6-9756-4CAB-95AC-E998FBCF8C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,9 +535,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>Internet</t>
-  </si>
-  <si>
     <t>Type of Service</t>
   </si>
   <si>
@@ -878,17 +875,27 @@
   </si>
   <si>
     <t>canva</t>
+  </si>
+  <si>
+    <t>NetworkOperations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1041,24 +1048,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1914,10 +1922,10 @@
   <dimension ref="A1:AD988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="J59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="J41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD69" sqref="AD69"/>
+      <selection pane="bottomRight" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1968,25 +1976,25 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>273</v>
+      </c>
+      <c r="J1" t="s">
         <v>274</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>275</v>
-      </c>
-      <c r="K1" t="s">
-        <v>276</v>
       </c>
       <c r="L1" t="s">
         <v>8</v>
       </c>
       <c r="M1" t="s">
+        <v>267</v>
+      </c>
+      <c r="N1" t="s">
         <v>268</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>269</v>
-      </c>
-      <c r="O1" t="s">
-        <v>270</v>
       </c>
       <c r="P1" t="s">
         <v>10</v>
@@ -1995,7 +2003,7 @@
         <v>11</v>
       </c>
       <c r="R1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="S1" t="s">
         <v>13</v>
@@ -2013,7 +2021,7 @@
         <v>17</v>
       </c>
       <c r="X1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>18</v>
@@ -2025,13 +2033,13 @@
         <v>20</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
@@ -2295,7 +2303,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B7" t="s">
         <v>132</v>
@@ -2351,10 +2359,10 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C8" t="s">
         <v>133</v>
@@ -2377,10 +2385,10 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C9" t="s">
         <v>133</v>
@@ -2450,10 +2458,10 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C11" t="s">
         <v>133</v>
@@ -2485,10 +2493,10 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>214</v>
+      </c>
+      <c r="B12" t="s">
         <v>215</v>
-      </c>
-      <c r="B12" t="s">
-        <v>216</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -2664,7 +2672,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B16" t="s">
         <v>162</v>
@@ -2746,10 +2754,10 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" t="s">
         <v>219</v>
-      </c>
-      <c r="B18" t="s">
-        <v>220</v>
       </c>
       <c r="C18" t="s">
         <v>44</v>
@@ -2814,7 +2822,7 @@
         <v>1</v>
       </c>
       <c r="Q19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="R19">
         <v>1</v>
@@ -2910,10 +2918,10 @@
     </row>
     <row r="22" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>216</v>
+      </c>
+      <c r="B22" t="s">
         <v>217</v>
-      </c>
-      <c r="B22" t="s">
-        <v>218</v>
       </c>
       <c r="C22" t="s">
         <v>44</v>
@@ -2936,10 +2944,10 @@
     </row>
     <row r="23" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" t="s">
         <v>221</v>
-      </c>
-      <c r="B23" t="s">
-        <v>222</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
@@ -2974,10 +2982,10 @@
     </row>
     <row r="24" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C24" t="s">
         <v>44</v>
@@ -3509,10 +3517,10 @@
     </row>
     <row r="35" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B35" t="s">
         <v>187</v>
-      </c>
-      <c r="B35" t="s">
-        <v>188</v>
       </c>
       <c r="C35" t="s">
         <v>140</v>
@@ -3559,16 +3567,16 @@
     </row>
     <row r="36" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>183</v>
+      </c>
+      <c r="B36" t="s">
         <v>184</v>
-      </c>
-      <c r="B36" t="s">
-        <v>185</v>
       </c>
       <c r="C36" t="s">
         <v>140</v>
       </c>
       <c r="D36" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E36" t="s">
         <v>46</v>
@@ -3724,10 +3732,10 @@
     </row>
     <row r="39" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39" t="s">
         <v>189</v>
-      </c>
-      <c r="B39" t="s">
-        <v>190</v>
       </c>
       <c r="C39" t="s">
         <v>140</v>
@@ -3783,7 +3791,7 @@
         <v>82</v>
       </c>
       <c r="C40" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D40" t="s">
         <v>82</v>
@@ -3836,7 +3844,7 @@
         <v>84</v>
       </c>
       <c r="C41" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D41" t="s">
         <v>85</v>
@@ -3892,7 +3900,7 @@
         <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D42" t="s">
         <v>88</v>
@@ -3951,7 +3959,7 @@
         <v>77</v>
       </c>
       <c r="C43" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D43" t="s">
         <v>79</v>
@@ -4010,7 +4018,7 @@
         <v>81</v>
       </c>
       <c r="C44" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D44" t="s">
         <v>80</v>
@@ -4066,13 +4074,13 @@
     </row>
     <row r="45" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B45" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C45" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F45">
         <v>8</v>
@@ -4110,13 +4118,13 @@
     </row>
     <row r="46" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B46" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C46" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F46">
         <v>7</v>
@@ -4148,16 +4156,16 @@
     </row>
     <row r="47" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>190</v>
+      </c>
+      <c r="B47" t="s">
         <v>191</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
+        <v>279</v>
+      </c>
+      <c r="D47" t="s">
         <v>192</v>
-      </c>
-      <c r="C47" t="s">
-        <v>165</v>
-      </c>
-      <c r="D47" t="s">
-        <v>193</v>
       </c>
       <c r="E47" t="s">
         <v>46</v>
@@ -4201,16 +4209,16 @@
     </row>
     <row r="48" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>193</v>
+      </c>
+      <c r="B48" t="s">
         <v>194</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D48" t="s">
         <v>195</v>
-      </c>
-      <c r="C48" t="s">
-        <v>165</v>
-      </c>
-      <c r="D48" t="s">
-        <v>196</v>
       </c>
       <c r="F48">
         <v>9</v>
@@ -4251,13 +4259,13 @@
     </row>
     <row r="49" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>198</v>
+      </c>
+      <c r="B49" t="s">
         <v>199</v>
       </c>
-      <c r="B49" t="s">
-        <v>200</v>
-      </c>
       <c r="C49" t="s">
-        <v>165</v>
+        <v>279</v>
       </c>
       <c r="F49">
         <v>8</v>
@@ -4295,13 +4303,13 @@
     </row>
     <row r="50" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>200</v>
+      </c>
+      <c r="B50" t="s">
         <v>201</v>
       </c>
-      <c r="B50" t="s">
-        <v>202</v>
-      </c>
       <c r="C50" t="s">
-        <v>165</v>
+        <v>279</v>
       </c>
       <c r="F50">
         <v>8</v>
@@ -4345,13 +4353,13 @@
     </row>
     <row r="51" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>196</v>
+      </c>
+      <c r="B51" t="s">
         <v>197</v>
       </c>
-      <c r="B51" t="s">
-        <v>198</v>
-      </c>
       <c r="C51" t="s">
-        <v>165</v>
+        <v>279</v>
       </c>
       <c r="F51">
         <v>6</v>
@@ -4389,13 +4397,13 @@
     </row>
     <row r="52" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>248</v>
+      </c>
+      <c r="B52" t="s">
         <v>249</v>
       </c>
-      <c r="B52" t="s">
-        <v>250</v>
-      </c>
       <c r="C52" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F52">
         <v>8</v>
@@ -4439,13 +4447,13 @@
     </row>
     <row r="53" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>250</v>
+      </c>
+      <c r="B53" t="s">
         <v>251</v>
       </c>
-      <c r="B53" t="s">
-        <v>252</v>
-      </c>
       <c r="C53" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F53">
         <v>8</v>
@@ -4483,13 +4491,13 @@
     </row>
     <row r="54" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>246</v>
+      </c>
+      <c r="B54" t="s">
         <v>247</v>
       </c>
-      <c r="B54" t="s">
-        <v>248</v>
-      </c>
       <c r="C54" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F54">
         <v>8</v>
@@ -4521,16 +4529,16 @@
     </row>
     <row r="55" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>180</v>
+      </c>
+      <c r="B55" t="s">
         <v>181</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>245</v>
+      </c>
+      <c r="E55" t="s">
         <v>182</v>
-      </c>
-      <c r="C55" t="s">
-        <v>246</v>
-      </c>
-      <c r="E55" t="s">
-        <v>183</v>
       </c>
       <c r="F55">
         <v>8</v>
@@ -4556,13 +4564,13 @@
     </row>
     <row r="56" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" t="s">
         <v>179</v>
       </c>
-      <c r="B56" t="s">
-        <v>180</v>
-      </c>
       <c r="C56" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E56" t="s">
         <v>46</v>
@@ -4688,10 +4696,10 @@
     </row>
     <row r="59" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>209</v>
+      </c>
+      <c r="B59" t="s">
         <v>210</v>
-      </c>
-      <c r="B59" t="s">
-        <v>211</v>
       </c>
       <c r="C59" t="s">
         <v>109</v>
@@ -4855,10 +4863,10 @@
     </row>
     <row r="63" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>239</v>
+      </c>
+      <c r="B63" t="s">
         <v>240</v>
-      </c>
-      <c r="B63" t="s">
-        <v>241</v>
       </c>
       <c r="C63" t="s">
         <v>109</v>
@@ -4896,7 +4904,7 @@
     </row>
     <row r="64" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B64" t="s">
         <v>126</v>
@@ -5002,10 +5010,10 @@
     </row>
     <row r="66" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C66" t="s">
         <v>114</v>
@@ -5164,10 +5172,10 @@
     </row>
     <row r="69" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>212</v>
+      </c>
+      <c r="B69" t="s">
         <v>213</v>
-      </c>
-      <c r="B69" t="s">
-        <v>214</v>
       </c>
       <c r="C69" t="s">
         <v>114</v>
@@ -5217,10 +5225,10 @@
     </row>
     <row r="70" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B70" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C70" t="s">
         <v>114</v>
@@ -5500,10 +5508,10 @@
     </row>
     <row r="75" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B75" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C75" t="s">
         <v>114</v>
@@ -6552,27 +6560,27 @@
         <v>20</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="Z1" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="AA1" s="5" t="s">
         <v>230</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
         <v>132</v>
@@ -6626,15 +6634,15 @@
         <v>129949</v>
       </c>
       <c r="Z2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AA2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
         <v>162</v>
@@ -6672,10 +6680,10 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>133</v>
@@ -6707,10 +6715,10 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>219</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>220</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>44</v>
@@ -6745,10 +6753,10 @@
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>133</v>
@@ -6789,10 +6797,10 @@
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>44</v>
@@ -6824,10 +6832,10 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>244</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>245</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>114</v>
@@ -6871,10 +6879,10 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>252</v>
+      </c>
+      <c r="B9" t="s">
         <v>253</v>
-      </c>
-      <c r="B9" t="s">
-        <v>254</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>114</v>
@@ -6903,13 +6911,13 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C10" t="s">
         <v>263</v>
-      </c>
-      <c r="C10" t="s">
-        <v>264</v>
       </c>
       <c r="X10" s="6">
         <v>42522</v>
@@ -6920,10 +6928,10 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>133</v>
@@ -6940,10 +6948,10 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>242</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>243</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>78</v>
@@ -6978,10 +6986,10 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>109</v>
@@ -7016,10 +7024,10 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" t="s">
         <v>265</v>
-      </c>
-      <c r="B14" t="s">
-        <v>266</v>
       </c>
       <c r="C14" t="s">
         <v>133</v>
@@ -7042,10 +7050,10 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C15" t="s">
         <v>114</v>
@@ -7074,13 +7082,13 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F16">
         <v>6</v>
@@ -7112,10 +7120,10 @@
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17" t="s">
         <v>238</v>
-      </c>
-      <c r="B17" t="s">
-        <v>239</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>78</v>
@@ -7126,7 +7134,7 @@
     </row>
     <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>126</v>
@@ -7176,10 +7184,10 @@
     </row>
     <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>114</v>
@@ -7229,10 +7237,10 @@
     </row>
     <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C20" t="s">
         <v>44</v>
@@ -7264,10 +7272,10 @@
     </row>
     <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>133</v>
@@ -7311,10 +7319,10 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>114</v>
@@ -7358,10 +7366,10 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
@@ -7375,10 +7383,10 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>218</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>44</v>
@@ -7407,10 +7415,10 @@
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>239</v>
+      </c>
+      <c r="B25" t="s">
         <v>240</v>
-      </c>
-      <c r="B25" t="s">
-        <v>241</v>
       </c>
       <c r="C25" t="s">
         <v>109</v>
@@ -7448,10 +7456,10 @@
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>78</v>
@@ -7535,7 +7543,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B4">
         <f>COUNTIF(Services!$C$2:$C$75,Count!A4)</f>
@@ -7553,7 +7561,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>279</v>
       </c>
       <c r="B6">
         <f>COUNTIF(Services!$C$2:$C$75,Count!A6)</f>
@@ -7607,7 +7615,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B12">
         <f>COUNTIF(Services!$C$2:$C$75,Count!A12)</f>
@@ -8627,10 +8635,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -8638,7 +8646,7 @@
         <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8646,7 +8654,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -8654,7 +8662,7 @@
         <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -8662,15 +8670,15 @@
         <v>63</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>165</v>
+        <v>279</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -8678,7 +8686,7 @@
         <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -8686,7 +8694,7 @@
         <v>109</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -8694,7 +8702,7 @@
         <v>140</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -8702,7 +8710,7 @@
         <v>133</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -8710,15 +8718,15 @@
         <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9804,7 +9812,7 @@
         <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -9897,7 +9905,7 @@
         <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D4" t="s">
         <v>92</v>
@@ -9932,7 +9940,7 @@
         <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D5" t="s">
         <v>106</v>
@@ -9964,7 +9972,7 @@
         <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D6" t="s">
         <v>99</v>
@@ -10002,21 +10010,21 @@
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B7" t="s">
         <v>238</v>
       </c>
-      <c r="B7" t="s">
-        <v>239</v>
-      </c>
       <c r="C7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B8" t="s">
         <v>253</v>
-      </c>
-      <c r="B8" t="s">
-        <v>254</v>
       </c>
       <c r="C8" t="s">
         <v>114</v>
@@ -10039,10 +10047,10 @@
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
@@ -10050,21 +10058,21 @@
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C10" t="s">
         <v>263</v>
-      </c>
-      <c r="C10" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B11" t="s">
         <v>265</v>
-      </c>
-      <c r="B11" t="s">
-        <v>266</v>
       </c>
       <c r="C11" t="s">
         <v>133</v>
@@ -10087,10 +10095,10 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C12" t="s">
         <v>133</v>
@@ -10144,7 +10152,7 @@
         <v>133</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C2" s="12">
         <v>10</v>
@@ -10158,7 +10166,7 @@
         <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -10172,7 +10180,7 @@
         <v>133</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C4" s="12">
         <v>8</v>
@@ -10186,15 +10194,15 @@
         <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C6" s="12">
         <v>6</v>
@@ -10208,7 +10216,7 @@
         <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -10222,7 +10230,7 @@
         <v>133</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C8" s="12">
         <v>9</v>
@@ -10236,7 +10244,7 @@
         <v>133</v>
       </c>
       <c r="B9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -10244,7 +10252,7 @@
         <v>44</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C10" s="12">
         <v>8</v>
@@ -10258,7 +10266,7 @@
         <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -10272,7 +10280,7 @@
         <v>44</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C12" s="12">
         <v>8</v>
@@ -10286,7 +10294,7 @@
         <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C13">
         <v>8</v>
@@ -10300,7 +10308,7 @@
         <v>44</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C14" s="12">
         <v>6</v>
@@ -10314,7 +10322,7 @@
         <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -10322,7 +10330,7 @@
         <v>78</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C16" s="12">
         <v>8</v>
@@ -10336,7 +10344,7 @@
         <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -10344,7 +10352,7 @@
         <v>78</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C18" s="12">
         <v>7</v>
@@ -10355,10 +10363,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -10366,7 +10374,7 @@
         <v>109</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C20" s="12">
         <v>8</v>
@@ -10380,7 +10388,7 @@
         <v>109</v>
       </c>
       <c r="B21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C21">
         <v>8</v>
@@ -10394,7 +10402,7 @@
         <v>114</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C22" s="12">
         <v>5</v>
@@ -10408,7 +10416,7 @@
         <v>114</v>
       </c>
       <c r="B23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C23">
         <v>6</v>
@@ -10422,7 +10430,7 @@
         <v>114</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C24" s="12">
         <v>6</v>
@@ -10436,7 +10444,7 @@
         <v>114</v>
       </c>
       <c r="B25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -10444,7 +10452,7 @@
         <v>114</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C26" s="13">
         <v>1</v>

</xml_diff>